<commit_message>
knn with position-specific models
</commit_message>
<xml_diff>
--- a/modelIterations.xlsx
+++ b/modelIterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrkawa\Documents\Berkeley\w207\fantasyFootballML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBD6B38-36BC-4A8C-92D6-1DBC1C6E8EAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DB7765-5375-4FFA-BDDE-2FDB243787C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
   <si>
     <t>Split by Position</t>
   </si>
@@ -120,13 +120,13 @@
     <t>Principle Component Analysis</t>
   </si>
   <si>
-    <t>Really</t>
-  </si>
-  <si>
-    <t>quite</t>
-  </si>
-  <si>
-    <t>bad.</t>
+    <t>51.7</t>
+  </si>
+  <si>
+    <t>67.7</t>
+  </si>
+  <si>
+    <t>-0.13</t>
   </si>
 </sst>
 </file>
@@ -740,7 +740,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -903,6 +903,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1259,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V32"/>
+  <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,25 +1280,24 @@
     <col min="5" max="5" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="12.7109375" style="1"/>
+    <col min="8" max="8" width="13" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13" style="5" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="12.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11"/>
       <c r="B1" s="12"/>
       <c r="C1" s="13"/>
@@ -1306,29 +1311,28 @@
         <v>27</v>
       </c>
       <c r="I1" s="50"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="49" t="s">
+      <c r="J1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="50"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="49" t="s">
+      <c r="K1" s="50"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="50"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="49" t="s">
+      <c r="N1" s="50"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="50"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="49" t="s">
+      <c r="Q1" s="50"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="U1" s="50"/>
-      <c r="V1" s="51"/>
-    </row>
-    <row r="2" spans="1:22" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="T1" s="50"/>
+      <c r="U1" s="51"/>
+    </row>
+    <row r="2" spans="1:21" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -1350,47 +1354,44 @@
       <c r="I2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="M2" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="N2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="O2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="P2" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="Q2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="18" t="s">
+      <c r="R2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="S2" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="17" t="s">
+      <c r="T2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="18" t="s">
+      <c r="U2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="T2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="U2" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="V2" s="18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
         <v>7</v>
       </c>
@@ -1408,21 +1409,20 @@
       <c r="G3" s="32"/>
       <c r="H3" s="31"/>
       <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="32"/>
       <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="32"/>
-      <c r="V3" s="33"/>
-    </row>
-    <row r="4" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P3" s="31"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="33"/>
+    </row>
+    <row r="4" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="47"/>
       <c r="B4" s="44"/>
       <c r="C4" s="21" t="s">
@@ -1436,21 +1436,20 @@
       <c r="G4" s="35"/>
       <c r="H4" s="34"/>
       <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="35"/>
       <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="35"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="34"/>
-      <c r="U4" s="35"/>
-      <c r="V4" s="36"/>
-    </row>
-    <row r="5" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P4" s="34"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="36"/>
+    </row>
+    <row r="5" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="47"/>
       <c r="B5" s="45"/>
       <c r="C5" s="23" t="s">
@@ -1464,21 +1463,20 @@
       <c r="G5" s="38"/>
       <c r="H5" s="37"/>
       <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="38"/>
       <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="39"/>
-      <c r="T5" s="37"/>
-      <c r="U5" s="38"/>
-      <c r="V5" s="39"/>
-    </row>
-    <row r="6" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P5" s="37"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="39"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="39"/>
+    </row>
+    <row r="6" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="47"/>
       <c r="B6" s="43" t="s">
         <v>21</v>
@@ -1496,21 +1494,20 @@
       <c r="G6" s="32"/>
       <c r="H6" s="31"/>
       <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="32"/>
       <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="32"/>
-      <c r="S6" s="33"/>
-      <c r="T6" s="31"/>
-      <c r="U6" s="32"/>
-      <c r="V6" s="33"/>
-    </row>
-    <row r="7" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P6" s="31"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="32"/>
+      <c r="U6" s="33"/>
+    </row>
+    <row r="7" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" s="44"/>
       <c r="C7" s="21" t="s">
@@ -1526,21 +1523,20 @@
       <c r="G7" s="35"/>
       <c r="H7" s="34"/>
       <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="35"/>
       <c r="O7" s="35"/>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="34"/>
-      <c r="R7" s="35"/>
-      <c r="S7" s="36"/>
-      <c r="T7" s="34"/>
-      <c r="U7" s="35"/>
-      <c r="V7" s="36"/>
-    </row>
-    <row r="8" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P7" s="34"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="36"/>
+      <c r="S7" s="34"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="36"/>
+    </row>
+    <row r="8" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="47"/>
       <c r="B8" s="45"/>
       <c r="C8" s="23" t="s">
@@ -1556,21 +1552,20 @@
       <c r="G8" s="38"/>
       <c r="H8" s="37"/>
       <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="38"/>
       <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="37"/>
-      <c r="R8" s="38"/>
-      <c r="S8" s="39"/>
-      <c r="T8" s="37"/>
-      <c r="U8" s="38"/>
-      <c r="V8" s="39"/>
-    </row>
-    <row r="9" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P8" s="37"/>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="39"/>
+      <c r="S8" s="37"/>
+      <c r="T8" s="38"/>
+      <c r="U8" s="39"/>
+    </row>
+    <row r="9" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="47"/>
       <c r="B9" s="43" t="s">
         <v>10</v>
@@ -1590,23 +1585,26 @@
       <c r="G9" s="25">
         <v>31.4</v>
       </c>
-      <c r="H9" s="20"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="20"/>
+      <c r="H9" s="20">
+        <v>31.4</v>
+      </c>
+      <c r="I9" s="25">
+        <v>31.5</v>
+      </c>
+      <c r="J9" s="20"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="25"/>
       <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="20"/>
-      <c r="U9" s="25"/>
-      <c r="V9" s="28"/>
-    </row>
-    <row r="10" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P9" s="20"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="28"/>
+    </row>
+    <row r="10" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="47"/>
       <c r="B10" s="44"/>
       <c r="C10" s="21" t="s">
@@ -1624,23 +1622,26 @@
       <c r="G10" s="26">
         <v>47.4</v>
       </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="22"/>
+      <c r="H10" s="22">
+        <v>46.8</v>
+      </c>
+      <c r="I10" s="26">
+        <v>47.2</v>
+      </c>
+      <c r="J10" s="22"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="26"/>
       <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="22"/>
-      <c r="U10" s="26"/>
-      <c r="V10" s="29"/>
-    </row>
-    <row r="11" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P10" s="22"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="26"/>
+      <c r="U10" s="29"/>
+    </row>
+    <row r="11" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="47"/>
       <c r="B11" s="45"/>
       <c r="C11" s="23" t="s">
@@ -1658,23 +1659,26 @@
       <c r="G11" s="27">
         <v>0.45</v>
       </c>
-      <c r="H11" s="24"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="24"/>
+      <c r="H11" s="24">
+        <v>0.46</v>
+      </c>
+      <c r="I11" s="27">
+        <v>0.45</v>
+      </c>
+      <c r="J11" s="24"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="27"/>
       <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="30"/>
-      <c r="T11" s="24"/>
-      <c r="U11" s="27"/>
-      <c r="V11" s="30"/>
-    </row>
-    <row r="12" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P11" s="24"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="27"/>
+      <c r="U11" s="30"/>
+    </row>
+    <row r="12" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47"/>
       <c r="B12" s="43" t="s">
         <v>11</v>
@@ -1694,23 +1698,26 @@
       <c r="G12" s="25">
         <v>31.7</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="20"/>
+      <c r="H12" s="20">
+        <v>31.4</v>
+      </c>
+      <c r="I12" s="25">
+        <v>31.5</v>
+      </c>
+      <c r="J12" s="20"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="25"/>
       <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="28"/>
-      <c r="T12" s="20"/>
-      <c r="U12" s="25"/>
-      <c r="V12" s="28"/>
-    </row>
-    <row r="13" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P12" s="20"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="25"/>
+      <c r="U12" s="28"/>
+    </row>
+    <row r="13" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47"/>
       <c r="B13" s="44"/>
       <c r="C13" s="21" t="s">
@@ -1728,23 +1735,26 @@
       <c r="G13" s="26">
         <v>47.4</v>
       </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="22"/>
+      <c r="H13" s="22">
+        <v>46.8</v>
+      </c>
+      <c r="I13" s="26">
+        <v>47.2</v>
+      </c>
+      <c r="J13" s="22"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="26"/>
       <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="26"/>
-      <c r="S13" s="29"/>
-      <c r="T13" s="22"/>
-      <c r="U13" s="26"/>
-      <c r="V13" s="29"/>
-    </row>
-    <row r="14" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P13" s="22"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="29"/>
+      <c r="S13" s="22"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="29"/>
+    </row>
+    <row r="14" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="47"/>
       <c r="B14" s="45"/>
       <c r="C14" s="23" t="s">
@@ -1762,23 +1772,26 @@
       <c r="G14" s="27">
         <v>0.45</v>
       </c>
-      <c r="H14" s="24"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="24"/>
+      <c r="H14" s="24">
+        <v>0.46</v>
+      </c>
+      <c r="I14" s="27">
+        <v>0.45</v>
+      </c>
+      <c r="J14" s="24"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="27"/>
       <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="27"/>
-      <c r="S14" s="30"/>
-      <c r="T14" s="24"/>
-      <c r="U14" s="27"/>
-      <c r="V14" s="30"/>
-    </row>
-    <row r="15" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P14" s="24"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="27"/>
+      <c r="U14" s="30"/>
+    </row>
+    <row r="15" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="47"/>
       <c r="B15" s="43" t="s">
         <v>9</v>
@@ -1800,21 +1813,20 @@
       </c>
       <c r="H15" s="31"/>
       <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="32"/>
       <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="31"/>
-      <c r="R15" s="32"/>
-      <c r="S15" s="33"/>
-      <c r="T15" s="31"/>
-      <c r="U15" s="32"/>
-      <c r="V15" s="33"/>
-    </row>
-    <row r="16" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P15" s="31"/>
+      <c r="Q15" s="32"/>
+      <c r="R15" s="33"/>
+      <c r="S15" s="31"/>
+      <c r="T15" s="32"/>
+      <c r="U15" s="33"/>
+    </row>
+    <row r="16" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="47"/>
       <c r="B16" s="44"/>
       <c r="C16" s="21" t="s">
@@ -1834,21 +1846,20 @@
       </c>
       <c r="H16" s="34"/>
       <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="35"/>
       <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="34"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="36"/>
-      <c r="T16" s="34"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="36"/>
-    </row>
-    <row r="17" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P16" s="34"/>
+      <c r="Q16" s="35"/>
+      <c r="R16" s="36"/>
+      <c r="S16" s="34"/>
+      <c r="T16" s="35"/>
+      <c r="U16" s="36"/>
+    </row>
+    <row r="17" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="48"/>
       <c r="B17" s="45"/>
       <c r="C17" s="23" t="s">
@@ -1868,21 +1879,20 @@
       </c>
       <c r="H17" s="37"/>
       <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="38"/>
       <c r="O17" s="38"/>
-      <c r="P17" s="38"/>
-      <c r="Q17" s="37"/>
-      <c r="R17" s="38"/>
-      <c r="S17" s="39"/>
-      <c r="T17" s="37"/>
-      <c r="U17" s="38"/>
-      <c r="V17" s="39"/>
-    </row>
-    <row r="18" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P17" s="37"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="39"/>
+      <c r="S17" s="37"/>
+      <c r="T17" s="38"/>
+      <c r="U17" s="39"/>
+    </row>
+    <row r="18" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
         <v>12</v>
       </c>
@@ -1898,7 +1908,7 @@
       <c r="E18" s="26">
         <v>29.9</v>
       </c>
-      <c r="F18" s="26" t="s">
+      <c r="F18" s="55" t="s">
         <v>30</v>
       </c>
       <c r="G18" s="26">
@@ -1906,21 +1916,20 @@
       </c>
       <c r="H18" s="34"/>
       <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="35"/>
       <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="34"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="36"/>
-      <c r="T18" s="34"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="36"/>
-    </row>
-    <row r="19" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P18" s="34"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="34"/>
+      <c r="T18" s="35"/>
+      <c r="U18" s="36"/>
+    </row>
+    <row r="19" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="44"/>
       <c r="C19" s="21" t="s">
@@ -1932,7 +1941,7 @@
       <c r="E19" s="26">
         <v>50.3</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="55" t="s">
         <v>31</v>
       </c>
       <c r="G19" s="26">
@@ -1940,21 +1949,20 @@
       </c>
       <c r="H19" s="34"/>
       <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="35"/>
       <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="34"/>
-      <c r="R19" s="35"/>
-      <c r="S19" s="36"/>
-      <c r="T19" s="34"/>
-      <c r="U19" s="35"/>
-      <c r="V19" s="36"/>
-    </row>
-    <row r="20" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P19" s="34"/>
+      <c r="Q19" s="35"/>
+      <c r="R19" s="36"/>
+      <c r="S19" s="34"/>
+      <c r="T19" s="35"/>
+      <c r="U19" s="36"/>
+    </row>
+    <row r="20" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="48"/>
       <c r="B20" s="45"/>
       <c r="C20" s="23" t="s">
@@ -1966,7 +1974,7 @@
       <c r="E20" s="27">
         <v>0.38</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="56" t="s">
         <v>32</v>
       </c>
       <c r="G20" s="27">
@@ -1974,21 +1982,20 @@
       </c>
       <c r="H20" s="37"/>
       <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="38"/>
       <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="37"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="39"/>
-      <c r="T20" s="37"/>
-      <c r="U20" s="38"/>
-      <c r="V20" s="39"/>
-    </row>
-    <row r="21" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P20" s="37"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="39"/>
+      <c r="S20" s="37"/>
+      <c r="T20" s="38"/>
+      <c r="U20" s="39"/>
+    </row>
+    <row r="21" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="46" t="s">
         <v>13</v>
       </c>
@@ -2010,23 +2017,26 @@
       <c r="G21" s="25">
         <v>31.3</v>
       </c>
-      <c r="H21" s="20"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="20"/>
+      <c r="H21" s="20">
+        <v>30.7</v>
+      </c>
+      <c r="I21" s="25">
+        <v>31.2</v>
+      </c>
+      <c r="J21" s="20"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="25"/>
       <c r="O21" s="25"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="28"/>
-      <c r="T21" s="20"/>
-      <c r="U21" s="25"/>
-      <c r="V21" s="28"/>
-    </row>
-    <row r="22" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P21" s="20"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="28"/>
+      <c r="S21" s="20"/>
+      <c r="T21" s="25"/>
+      <c r="U21" s="28"/>
+    </row>
+    <row r="22" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="47"/>
       <c r="B22" s="44"/>
       <c r="C22" s="21" t="s">
@@ -2044,23 +2054,26 @@
       <c r="G22" s="26">
         <v>47.3</v>
       </c>
-      <c r="H22" s="22"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="22"/>
+      <c r="H22" s="22">
+        <v>48.8</v>
+      </c>
+      <c r="I22" s="26">
+        <v>47.2</v>
+      </c>
+      <c r="J22" s="22"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="26"/>
       <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="26"/>
-      <c r="S22" s="29"/>
-      <c r="T22" s="22"/>
-      <c r="U22" s="26"/>
-      <c r="V22" s="29"/>
-    </row>
-    <row r="23" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P22" s="22"/>
+      <c r="Q22" s="26"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="22"/>
+      <c r="T22" s="26"/>
+      <c r="U22" s="29"/>
+    </row>
+    <row r="23" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="48"/>
       <c r="B23" s="45"/>
       <c r="C23" s="23" t="s">
@@ -2078,23 +2091,26 @@
       <c r="G23" s="27">
         <v>0.45</v>
       </c>
-      <c r="H23" s="24"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="24"/>
+      <c r="H23" s="24">
+        <v>0.41</v>
+      </c>
+      <c r="I23" s="27">
+        <v>0.45</v>
+      </c>
+      <c r="J23" s="24"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="27"/>
       <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="27"/>
-      <c r="S23" s="30"/>
-      <c r="T23" s="24"/>
-      <c r="U23" s="27"/>
-      <c r="V23" s="30"/>
-    </row>
-    <row r="24" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P23" s="24"/>
+      <c r="Q23" s="27"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="24"/>
+      <c r="T23" s="27"/>
+      <c r="U23" s="30"/>
+    </row>
+    <row r="24" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="46" t="s">
         <v>15</v>
       </c>
@@ -2110,7 +2126,9 @@
       <c r="E24" s="25">
         <v>31</v>
       </c>
-      <c r="F24" s="25"/>
+      <c r="F24" s="25">
+        <v>31.7</v>
+      </c>
       <c r="G24" s="40">
         <v>31.8</v>
       </c>
@@ -2120,21 +2138,20 @@
       <c r="I24" s="25">
         <v>31.2</v>
       </c>
-      <c r="J24" s="25"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="25"/>
       <c r="O24" s="25"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="20"/>
-      <c r="R24" s="25"/>
-      <c r="S24" s="28"/>
-      <c r="T24" s="20"/>
-      <c r="U24" s="25"/>
-      <c r="V24" s="28"/>
-    </row>
-    <row r="25" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P24" s="20"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="28"/>
+      <c r="S24" s="20"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="28"/>
+    </row>
+    <row r="25" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47"/>
       <c r="B25" s="44"/>
       <c r="C25" s="21" t="s">
@@ -2146,7 +2163,9 @@
       <c r="E25" s="26">
         <v>47.1</v>
       </c>
-      <c r="F25" s="26"/>
+      <c r="F25" s="26">
+        <v>47.4</v>
+      </c>
       <c r="G25" s="41">
         <v>47.1</v>
       </c>
@@ -2156,21 +2175,20 @@
       <c r="I25" s="26">
         <v>46.7</v>
       </c>
-      <c r="J25" s="26"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="26"/>
       <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="22"/>
-      <c r="R25" s="26"/>
-      <c r="S25" s="29"/>
-      <c r="T25" s="22"/>
-      <c r="U25" s="26"/>
-      <c r="V25" s="29"/>
-    </row>
-    <row r="26" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P25" s="22"/>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="29"/>
+      <c r="S25" s="22"/>
+      <c r="T25" s="26"/>
+      <c r="U25" s="29"/>
+    </row>
+    <row r="26" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="48"/>
       <c r="B26" s="45"/>
       <c r="C26" s="23" t="s">
@@ -2182,7 +2200,9 @@
       <c r="E26" s="27">
         <v>0.45</v>
       </c>
-      <c r="F26" s="27"/>
+      <c r="F26" s="27">
+        <v>0.45</v>
+      </c>
       <c r="G26" s="42">
         <v>0.45</v>
       </c>
@@ -2192,21 +2212,20 @@
       <c r="I26" s="27">
         <v>0.46</v>
       </c>
-      <c r="J26" s="27"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="30"/>
-      <c r="N26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="27"/>
       <c r="O26" s="27"/>
-      <c r="P26" s="27"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="27"/>
-      <c r="S26" s="30"/>
-      <c r="T26" s="24"/>
-      <c r="U26" s="27"/>
-      <c r="V26" s="30"/>
-    </row>
-    <row r="27" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P26" s="24"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="24"/>
+      <c r="T26" s="27"/>
+      <c r="U26" s="30"/>
+    </row>
+    <row r="27" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="52" t="s">
         <v>17</v>
       </c>
@@ -2222,21 +2241,20 @@
       <c r="G27" s="25"/>
       <c r="H27" s="20"/>
       <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="25"/>
       <c r="O27" s="25"/>
-      <c r="P27" s="25"/>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="25"/>
-      <c r="S27" s="28"/>
-      <c r="T27" s="20"/>
-      <c r="U27" s="25"/>
-      <c r="V27" s="28"/>
-    </row>
-    <row r="28" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P27" s="20"/>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="28"/>
+      <c r="S27" s="20"/>
+      <c r="T27" s="25"/>
+      <c r="U27" s="28"/>
+    </row>
+    <row r="28" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="53"/>
       <c r="B28" s="44"/>
       <c r="C28" s="21" t="s">
@@ -2248,21 +2266,20 @@
       <c r="G28" s="26"/>
       <c r="H28" s="22"/>
       <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="26"/>
       <c r="O28" s="26"/>
-      <c r="P28" s="26"/>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="26"/>
-      <c r="S28" s="29"/>
-      <c r="T28" s="22"/>
-      <c r="U28" s="26"/>
-      <c r="V28" s="29"/>
-    </row>
-    <row r="29" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P28" s="22"/>
+      <c r="Q28" s="26"/>
+      <c r="R28" s="29"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="26"/>
+      <c r="U28" s="29"/>
+    </row>
+    <row r="29" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="53"/>
       <c r="B29" s="45"/>
       <c r="C29" s="23" t="s">
@@ -2274,21 +2291,20 @@
       <c r="G29" s="27"/>
       <c r="H29" s="24"/>
       <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="30"/>
-      <c r="N29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="27"/>
       <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="30"/>
-      <c r="T29" s="24"/>
-      <c r="U29" s="27"/>
-      <c r="V29" s="30"/>
-    </row>
-    <row r="30" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P29" s="24"/>
+      <c r="Q29" s="27"/>
+      <c r="R29" s="30"/>
+      <c r="S29" s="24"/>
+      <c r="T29" s="27"/>
+      <c r="U29" s="30"/>
+    </row>
+    <row r="30" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="53"/>
       <c r="B30" s="44" t="s">
         <v>19</v>
@@ -2302,21 +2318,20 @@
       <c r="G30" s="26"/>
       <c r="H30" s="22"/>
       <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="26"/>
       <c r="O30" s="26"/>
-      <c r="P30" s="26"/>
-      <c r="Q30" s="22"/>
-      <c r="R30" s="26"/>
-      <c r="S30" s="29"/>
-      <c r="T30" s="22"/>
-      <c r="U30" s="26"/>
-      <c r="V30" s="29"/>
-    </row>
-    <row r="31" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P30" s="22"/>
+      <c r="Q30" s="26"/>
+      <c r="R30" s="29"/>
+      <c r="S30" s="22"/>
+      <c r="T30" s="26"/>
+      <c r="U30" s="29"/>
+    </row>
+    <row r="31" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="53"/>
       <c r="B31" s="44"/>
       <c r="C31" s="21" t="s">
@@ -2328,21 +2343,20 @@
       <c r="G31" s="26"/>
       <c r="H31" s="22"/>
       <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="22"/>
+      <c r="N31" s="26"/>
       <c r="O31" s="26"/>
-      <c r="P31" s="26"/>
-      <c r="Q31" s="22"/>
-      <c r="R31" s="26"/>
-      <c r="S31" s="29"/>
-      <c r="T31" s="22"/>
-      <c r="U31" s="26"/>
-      <c r="V31" s="29"/>
-    </row>
-    <row r="32" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P31" s="22"/>
+      <c r="Q31" s="26"/>
+      <c r="R31" s="29"/>
+      <c r="S31" s="22"/>
+      <c r="T31" s="26"/>
+      <c r="U31" s="29"/>
+    </row>
+    <row r="32" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="54"/>
       <c r="B32" s="45"/>
       <c r="C32" s="23" t="s">
@@ -2354,30 +2368,29 @@
       <c r="G32" s="27"/>
       <c r="H32" s="24"/>
       <c r="I32" s="27"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="27"/>
-      <c r="M32" s="30"/>
-      <c r="N32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="27"/>
+      <c r="L32" s="30"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="27"/>
       <c r="O32" s="27"/>
-      <c r="P32" s="27"/>
-      <c r="Q32" s="24"/>
-      <c r="R32" s="27"/>
-      <c r="S32" s="30"/>
-      <c r="T32" s="24"/>
-      <c r="U32" s="27"/>
-      <c r="V32" s="30"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="27"/>
+      <c r="R32" s="30"/>
+      <c r="S32" s="24"/>
+      <c r="T32" s="27"/>
+      <c r="U32" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="S1:U1"/>
     <mergeCell ref="A27:A32"/>
     <mergeCell ref="D1:G1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="J1:L1"/>
     <mergeCell ref="A24:A26"/>
-    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H1:I1"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="B9:B11"/>
@@ -2438,5 +2451,8 @@
     <firstHeader>&amp;C_x000D__x000D__x000D_</firstHeader>
     <firstFooter>&amp;C_x000D__x000D__x000D_</firstFooter>
   </headerFooter>
+  <ignoredErrors>
+    <ignoredError sqref="F18:F20" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed QB point calc
</commit_message>
<xml_diff>
--- a/modelIterations.xlsx
+++ b/modelIterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrkawa\Documents\Berkeley\w207\fantasyFootballML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DB7765-5375-4FFA-BDDE-2FDB243787C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AAF593-D88A-414B-B987-CAF39338D557}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="modelIterations" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -868,6 +869,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -876,39 +910,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1301,36 +1302,36 @@
       <c r="A1" s="11"/>
       <c r="B1" s="12"/>
       <c r="C1" s="13"/>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="49" t="s">
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="50"/>
-      <c r="J1" s="49" t="s">
+      <c r="I1" s="46"/>
+      <c r="J1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="50"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="49" t="s">
+      <c r="K1" s="46"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="50"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="49" t="s">
+      <c r="N1" s="46"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="49" t="s">
+      <c r="Q1" s="46"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="50"/>
-      <c r="U1" s="51"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="47"/>
     </row>
     <row r="2" spans="1:21" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
@@ -1392,10 +1393,10 @@
       </c>
     </row>
     <row r="3" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="54" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="19" t="s">
@@ -1423,8 +1424,8 @@
       <c r="U3" s="33"/>
     </row>
     <row r="4" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="44"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="21" t="s">
         <v>24</v>
       </c>
@@ -1450,8 +1451,8 @@
       <c r="U4" s="36"/>
     </row>
     <row r="5" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="45"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="56"/>
       <c r="C5" s="23" t="s">
         <v>23</v>
       </c>
@@ -1477,8 +1478,8 @@
       <c r="U5" s="39"/>
     </row>
     <row r="6" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="43" t="s">
+      <c r="A6" s="52"/>
+      <c r="B6" s="54" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="19" t="s">
@@ -1508,8 +1509,8 @@
       <c r="U6" s="33"/>
     </row>
     <row r="7" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="44"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="21" t="s">
         <v>24</v>
       </c>
@@ -1537,8 +1538,8 @@
       <c r="U7" s="36"/>
     </row>
     <row r="8" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="45"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="23" t="s">
         <v>23</v>
       </c>
@@ -1566,8 +1567,8 @@
       <c r="U8" s="39"/>
     </row>
     <row r="9" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="43" t="s">
+      <c r="A9" s="52"/>
+      <c r="B9" s="54" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="19" t="s">
@@ -1605,8 +1606,8 @@
       <c r="U9" s="28"/>
     </row>
     <row r="10" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="44"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="21" t="s">
         <v>24</v>
       </c>
@@ -1642,8 +1643,8 @@
       <c r="U10" s="29"/>
     </row>
     <row r="11" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="45"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="23" t="s">
         <v>23</v>
       </c>
@@ -1679,8 +1680,8 @@
       <c r="U11" s="30"/>
     </row>
     <row r="12" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
-      <c r="B12" s="43" t="s">
+      <c r="A12" s="52"/>
+      <c r="B12" s="54" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="19" t="s">
@@ -1718,8 +1719,8 @@
       <c r="U12" s="28"/>
     </row>
     <row r="13" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
-      <c r="B13" s="44"/>
+      <c r="A13" s="52"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="21" t="s">
         <v>24</v>
       </c>
@@ -1755,8 +1756,8 @@
       <c r="U13" s="29"/>
     </row>
     <row r="14" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="45"/>
+      <c r="A14" s="52"/>
+      <c r="B14" s="56"/>
       <c r="C14" s="23" t="s">
         <v>23</v>
       </c>
@@ -1792,8 +1793,8 @@
       <c r="U14" s="30"/>
     </row>
     <row r="15" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="43" t="s">
+      <c r="A15" s="52"/>
+      <c r="B15" s="54" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="19" t="s">
@@ -1827,8 +1828,8 @@
       <c r="U15" s="33"/>
     </row>
     <row r="16" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
-      <c r="B16" s="44"/>
+      <c r="A16" s="52"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="21" t="s">
         <v>24</v>
       </c>
@@ -1860,8 +1861,8 @@
       <c r="U16" s="36"/>
     </row>
     <row r="17" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
-      <c r="B17" s="45"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="23" t="s">
         <v>23</v>
       </c>
@@ -1893,10 +1894,10 @@
       <c r="U17" s="39"/>
     </row>
     <row r="18" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="54" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="21" t="s">
@@ -1908,7 +1909,7 @@
       <c r="E18" s="26">
         <v>29.9</v>
       </c>
-      <c r="F18" s="55" t="s">
+      <c r="F18" s="43" t="s">
         <v>30</v>
       </c>
       <c r="G18" s="26">
@@ -1930,8 +1931,8 @@
       <c r="U18" s="36"/>
     </row>
     <row r="19" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="44"/>
+      <c r="A19" s="52"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="21" t="s">
         <v>24</v>
       </c>
@@ -1941,7 +1942,7 @@
       <c r="E19" s="26">
         <v>50.3</v>
       </c>
-      <c r="F19" s="55" t="s">
+      <c r="F19" s="43" t="s">
         <v>31</v>
       </c>
       <c r="G19" s="26">
@@ -1963,8 +1964,8 @@
       <c r="U19" s="36"/>
     </row>
     <row r="20" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="48"/>
-      <c r="B20" s="45"/>
+      <c r="A20" s="53"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="23" t="s">
         <v>23</v>
       </c>
@@ -1974,7 +1975,7 @@
       <c r="E20" s="27">
         <v>0.38</v>
       </c>
-      <c r="F20" s="56" t="s">
+      <c r="F20" s="44" t="s">
         <v>32</v>
       </c>
       <c r="G20" s="27">
@@ -1996,10 +1997,10 @@
       <c r="U20" s="39"/>
     </row>
     <row r="21" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="54" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="19" t="s">
@@ -2037,8 +2038,8 @@
       <c r="U21" s="28"/>
     </row>
     <row r="22" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
-      <c r="B22" s="44"/>
+      <c r="A22" s="52"/>
+      <c r="B22" s="55"/>
       <c r="C22" s="21" t="s">
         <v>24</v>
       </c>
@@ -2074,8 +2075,8 @@
       <c r="U22" s="29"/>
     </row>
     <row r="23" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="48"/>
-      <c r="B23" s="45"/>
+      <c r="A23" s="53"/>
+      <c r="B23" s="56"/>
       <c r="C23" s="23" t="s">
         <v>23</v>
       </c>
@@ -2111,10 +2112,10 @@
       <c r="U23" s="30"/>
     </row>
     <row r="24" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="54" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="19" t="s">
@@ -2152,8 +2153,8 @@
       <c r="U24" s="28"/>
     </row>
     <row r="25" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="44"/>
+      <c r="A25" s="52"/>
+      <c r="B25" s="55"/>
       <c r="C25" s="21" t="s">
         <v>24</v>
       </c>
@@ -2189,8 +2190,8 @@
       <c r="U25" s="29"/>
     </row>
     <row r="26" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="48"/>
-      <c r="B26" s="45"/>
+      <c r="A26" s="53"/>
+      <c r="B26" s="56"/>
       <c r="C26" s="23" t="s">
         <v>23</v>
       </c>
@@ -2226,10 +2227,10 @@
       <c r="U26" s="30"/>
     </row>
     <row r="27" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="52" t="s">
+      <c r="A27" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="54" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="19" t="s">
@@ -2255,8 +2256,8 @@
       <c r="U27" s="28"/>
     </row>
     <row r="28" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="53"/>
-      <c r="B28" s="44"/>
+      <c r="A28" s="49"/>
+      <c r="B28" s="55"/>
       <c r="C28" s="21" t="s">
         <v>24</v>
       </c>
@@ -2280,8 +2281,8 @@
       <c r="U28" s="29"/>
     </row>
     <row r="29" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
-      <c r="B29" s="45"/>
+      <c r="A29" s="49"/>
+      <c r="B29" s="56"/>
       <c r="C29" s="23" t="s">
         <v>23</v>
       </c>
@@ -2305,8 +2306,8 @@
       <c r="U29" s="30"/>
     </row>
     <row r="30" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="53"/>
-      <c r="B30" s="44" t="s">
+      <c r="A30" s="49"/>
+      <c r="B30" s="55" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="21" t="s">
@@ -2332,8 +2333,8 @@
       <c r="U30" s="29"/>
     </row>
     <row r="31" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="53"/>
-      <c r="B31" s="44"/>
+      <c r="A31" s="49"/>
+      <c r="B31" s="55"/>
       <c r="C31" s="21" t="s">
         <v>24</v>
       </c>
@@ -2357,8 +2358,8 @@
       <c r="U31" s="29"/>
     </row>
     <row r="32" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
-      <c r="B32" s="45"/>
+      <c r="A32" s="50"/>
+      <c r="B32" s="56"/>
       <c r="C32" s="23" t="s">
         <v>23</v>
       </c>
@@ -2383,6 +2384,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A18:A20"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="A27:A32"/>
     <mergeCell ref="D1:G1"/>
@@ -2399,11 +2405,6 @@
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="A3:A17"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A18:A20"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:XFD3 A6:XFD6 A9:XFD9 A12:XFD12 A18:XFD18 A15:XFD15 A21:XFD21 A24:XFD24 A27:XFD27 A30:XFD30">
     <cfRule type="colorScale" priority="4">

</xml_diff>

<commit_message>
updates to tracker sheet
</commit_message>
<xml_diff>
--- a/modelIterations.xlsx
+++ b/modelIterations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrkawa\Documents\Berkeley\w207\fantasyFootballML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AAF593-D88A-414B-B987-CAF39338D557}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A49F719-0617-41DF-9D95-C56C2590B9CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-4680" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modelIterations" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="39">
   <si>
     <t>Split by Position</t>
   </si>
@@ -128,6 +128,24 @@
   </si>
   <si>
     <t>-0.13</t>
+  </si>
+  <si>
+    <t>Base Model</t>
+  </si>
+  <si>
+    <t>QB</t>
+  </si>
+  <si>
+    <t>RB</t>
+  </si>
+  <si>
+    <t>WR</t>
+  </si>
+  <si>
+    <t>TE</t>
+  </si>
+  <si>
+    <t>Downselected Features</t>
   </si>
 </sst>
 </file>
@@ -741,17 +759,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -761,9 +770,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -869,6 +875,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -910,6 +919,30 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1266,1148 +1299,1692 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U32"/>
+  <dimension ref="A1:AD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13" style="5" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="12.7109375" style="1"/>
+    <col min="1" max="1" width="14.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="26" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="12.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="45" t="s">
+    <row r="1" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="45" t="s">
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="45" t="s">
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="46"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="45" t="s">
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="45" t="s">
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="45" t="s">
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="46"/>
-      <c r="U1" s="47"/>
-    </row>
-    <row r="2" spans="1:21" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16" t="s">
+      <c r="AD1" s="44"/>
+    </row>
+    <row r="2" spans="1:30" s="1" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="J2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="K2" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="18" t="s">
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="52"/>
+      <c r="S2" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="X2" s="56"/>
+      <c r="Y2" s="56"/>
+      <c r="Z2" s="52"/>
+      <c r="AA2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="AC2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="O2" s="18" t="s">
+      <c r="AD2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="R2" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="T2" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="U2" s="18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+    </row>
+    <row r="3" spans="1:30" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="54"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="T3" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="U3" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="V3" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="W3" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="X3" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y3" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z3" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA3" s="54"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="54"/>
+      <c r="AD3" s="39"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B4" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C4" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D4" s="16">
         <v>31.7</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="31"/>
-      <c r="T3" s="32"/>
-      <c r="U3" s="33"/>
-    </row>
-    <row r="4" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="21" t="s">
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="28"/>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="28"/>
+      <c r="Z4" s="28"/>
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="28"/>
+      <c r="AD4" s="29"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="49"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D5" s="18">
         <v>47.1</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="34"/>
-      <c r="T4" s="35"/>
-      <c r="U4" s="36"/>
-    </row>
-    <row r="5" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="23" t="s">
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
+      <c r="V5" s="31"/>
+      <c r="W5" s="31"/>
+      <c r="X5" s="31"/>
+      <c r="Y5" s="31"/>
+      <c r="Z5" s="31"/>
+      <c r="AA5" s="31"/>
+      <c r="AB5" s="31"/>
+      <c r="AC5" s="31"/>
+      <c r="AD5" s="32"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="49"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D6" s="20">
         <v>0.45</v>
       </c>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="37"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="39"/>
-    </row>
-    <row r="6" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
-      <c r="B6" s="54" t="s">
+      <c r="E6" s="34"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="31"/>
+      <c r="V6" s="31"/>
+      <c r="W6" s="31"/>
+      <c r="X6" s="31"/>
+      <c r="Y6" s="31"/>
+      <c r="Z6" s="31"/>
+      <c r="AA6" s="31"/>
+      <c r="AB6" s="31"/>
+      <c r="AC6" s="31"/>
+      <c r="AD6" s="32"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="49"/>
+      <c r="B7" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D7" s="16">
         <v>31.7</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E7" s="21">
         <v>31.6</v>
       </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="31"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="33"/>
-    </row>
-    <row r="7" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="21" t="s">
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="31"/>
+      <c r="V7" s="31"/>
+      <c r="W7" s="31"/>
+      <c r="X7" s="31"/>
+      <c r="Y7" s="31"/>
+      <c r="Z7" s="31"/>
+      <c r="AA7" s="31"/>
+      <c r="AB7" s="31"/>
+      <c r="AC7" s="31"/>
+      <c r="AD7" s="32"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" s="49"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D8" s="18">
         <v>47.4</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E8" s="22">
         <v>47.3</v>
       </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="36"/>
-      <c r="S7" s="34"/>
-      <c r="T7" s="35"/>
-      <c r="U7" s="36"/>
-    </row>
-    <row r="8" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="56"/>
-      <c r="C8" s="23" t="s">
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="31"/>
+      <c r="U8" s="31"/>
+      <c r="V8" s="31"/>
+      <c r="W8" s="31"/>
+      <c r="X8" s="31"/>
+      <c r="Y8" s="31"/>
+      <c r="Z8" s="31"/>
+      <c r="AA8" s="31"/>
+      <c r="AB8" s="31"/>
+      <c r="AC8" s="31"/>
+      <c r="AD8" s="32"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" s="49"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D9" s="20">
         <v>0.45</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E9" s="23">
         <v>0.45</v>
       </c>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="37"/>
-      <c r="T8" s="38"/>
-      <c r="U8" s="39"/>
-    </row>
-    <row r="9" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="54" t="s">
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="34"/>
+      <c r="T9" s="34"/>
+      <c r="U9" s="34"/>
+      <c r="V9" s="34"/>
+      <c r="W9" s="34"/>
+      <c r="X9" s="34"/>
+      <c r="Y9" s="34"/>
+      <c r="Z9" s="34"/>
+      <c r="AA9" s="34"/>
+      <c r="AB9" s="34"/>
+      <c r="AC9" s="34"/>
+      <c r="AD9" s="35"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A10" s="49"/>
+      <c r="B10" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D10" s="16">
         <v>31.6</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E10" s="21">
         <v>31.8</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F10" s="21">
         <v>31.8</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G10" s="21">
         <v>31.4</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H10" s="16">
+        <v>31.6</v>
+      </c>
+      <c r="I10" s="21">
         <v>31.4</v>
       </c>
-      <c r="I9" s="25">
+      <c r="J10" s="21">
         <v>31.5</v>
       </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="28"/>
-    </row>
-    <row r="10" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="21" t="s">
+      <c r="K10" s="16">
+        <v>61.6</v>
+      </c>
+      <c r="L10" s="21">
+        <v>44.2</v>
+      </c>
+      <c r="M10" s="21">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="N10" s="21">
+        <v>20.9</v>
+      </c>
+      <c r="O10" s="21">
+        <v>61.9</v>
+      </c>
+      <c r="P10" s="21">
+        <v>44.3</v>
+      </c>
+      <c r="Q10" s="21">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="R10" s="24">
+        <v>20.9</v>
+      </c>
+      <c r="S10" s="16"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="21"/>
+      <c r="Z10" s="24"/>
+      <c r="AA10" s="16"/>
+      <c r="AB10" s="24"/>
+      <c r="AC10" s="16"/>
+      <c r="AD10" s="24"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" s="49"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D11" s="18">
         <v>47.3</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E11" s="22">
         <v>47.4</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F11" s="22">
         <v>47.4</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G11" s="22">
         <v>47.4</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H11" s="18">
+        <v>47.2</v>
+      </c>
+      <c r="I11" s="22">
         <v>46.8</v>
       </c>
-      <c r="I10" s="26">
+      <c r="J11" s="22">
         <v>47.2</v>
       </c>
-      <c r="J10" s="22"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="22"/>
-      <c r="T10" s="26"/>
-      <c r="U10" s="29"/>
-    </row>
-    <row r="11" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="23" t="s">
+      <c r="K11" s="18">
+        <v>81.8</v>
+      </c>
+      <c r="L11" s="22">
+        <v>61.6</v>
+      </c>
+      <c r="M11" s="22">
+        <v>55</v>
+      </c>
+      <c r="N11" s="22">
+        <v>29.5</v>
+      </c>
+      <c r="O11" s="22">
+        <v>81.5</v>
+      </c>
+      <c r="P11" s="22">
+        <v>61.6</v>
+      </c>
+      <c r="Q11" s="22">
+        <v>54.9</v>
+      </c>
+      <c r="R11" s="25">
+        <v>29.7</v>
+      </c>
+      <c r="S11" s="18"/>
+      <c r="T11" s="22"/>
+      <c r="U11" s="22"/>
+      <c r="V11" s="22"/>
+      <c r="W11" s="22"/>
+      <c r="X11" s="22"/>
+      <c r="Y11" s="22"/>
+      <c r="Z11" s="25"/>
+      <c r="AA11" s="18"/>
+      <c r="AB11" s="25"/>
+      <c r="AC11" s="18"/>
+      <c r="AD11" s="25"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="49"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D12" s="20">
         <v>0.45</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E12" s="23">
         <v>0.45</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F12" s="23">
         <v>0.45</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G12" s="23">
         <v>0.45</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H12" s="20">
+        <v>0.45</v>
+      </c>
+      <c r="I12" s="23">
         <v>0.46</v>
       </c>
-      <c r="I11" s="27">
+      <c r="J12" s="23">
         <v>0.45</v>
       </c>
-      <c r="J11" s="24"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="27"/>
-      <c r="U11" s="30"/>
-    </row>
-    <row r="12" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="52"/>
-      <c r="B12" s="54" t="s">
+      <c r="K12" s="20">
+        <v>0.43</v>
+      </c>
+      <c r="L12" s="23">
+        <v>0.43</v>
+      </c>
+      <c r="M12" s="23">
+        <v>0.43</v>
+      </c>
+      <c r="N12" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="O12" s="23">
+        <v>0.44</v>
+      </c>
+      <c r="P12" s="23">
+        <v>0.43</v>
+      </c>
+      <c r="Q12" s="23">
+        <v>0.43</v>
+      </c>
+      <c r="R12" s="26">
+        <v>0.49</v>
+      </c>
+      <c r="S12" s="20"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="23"/>
+      <c r="X12" s="23"/>
+      <c r="Y12" s="23"/>
+      <c r="Z12" s="26"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="26"/>
+      <c r="AC12" s="20"/>
+      <c r="AD12" s="26"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" s="49"/>
+      <c r="B13" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C13" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D13" s="16">
         <v>31.6</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E13" s="21">
         <v>31.6</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F13" s="21">
         <v>31.7</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G13" s="21">
         <v>31.7</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H13" s="16">
+        <v>31.6</v>
+      </c>
+      <c r="I13" s="21">
         <v>31.4</v>
       </c>
-      <c r="I12" s="25">
+      <c r="J13" s="21">
         <v>31.5</v>
       </c>
-      <c r="J12" s="20"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="20"/>
-      <c r="T12" s="25"/>
-      <c r="U12" s="28"/>
-    </row>
-    <row r="13" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="21" t="s">
+      <c r="K13" s="18">
+        <v>61.9</v>
+      </c>
+      <c r="L13" s="22">
+        <v>44.3</v>
+      </c>
+      <c r="M13" s="22">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="N13" s="22">
+        <v>20.9</v>
+      </c>
+      <c r="O13" s="22">
+        <v>31.9</v>
+      </c>
+      <c r="P13" s="22">
+        <v>44.3</v>
+      </c>
+      <c r="Q13" s="22">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="R13" s="25">
+        <v>20.9</v>
+      </c>
+      <c r="S13" s="18"/>
+      <c r="T13" s="22"/>
+      <c r="U13" s="22"/>
+      <c r="V13" s="22"/>
+      <c r="W13" s="22"/>
+      <c r="X13" s="22"/>
+      <c r="Y13" s="22"/>
+      <c r="Z13" s="25"/>
+      <c r="AA13" s="16"/>
+      <c r="AB13" s="24"/>
+      <c r="AC13" s="16"/>
+      <c r="AD13" s="24"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" s="49"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D14" s="18">
         <v>47.3</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E14" s="22">
         <v>47.3</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F14" s="22">
         <v>47.2</v>
       </c>
-      <c r="G13" s="26">
+      <c r="G14" s="22">
         <v>47.4</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H14" s="18">
+        <v>47.2</v>
+      </c>
+      <c r="I14" s="22">
         <v>46.8</v>
       </c>
-      <c r="I13" s="26">
+      <c r="J14" s="22">
         <v>47.2</v>
       </c>
-      <c r="J13" s="22"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="29"/>
-      <c r="S13" s="22"/>
-      <c r="T13" s="26"/>
-      <c r="U13" s="29"/>
-    </row>
-    <row r="14" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
-      <c r="B14" s="56"/>
-      <c r="C14" s="23" t="s">
+      <c r="K14" s="18">
+        <v>81.5</v>
+      </c>
+      <c r="L14" s="22">
+        <v>61.6</v>
+      </c>
+      <c r="M14" s="22">
+        <v>54.9</v>
+      </c>
+      <c r="N14" s="22">
+        <v>29.7</v>
+      </c>
+      <c r="O14" s="22">
+        <v>81.5</v>
+      </c>
+      <c r="P14" s="22">
+        <v>61.6</v>
+      </c>
+      <c r="Q14" s="22">
+        <v>54.9</v>
+      </c>
+      <c r="R14" s="25">
+        <v>29.7</v>
+      </c>
+      <c r="S14" s="18"/>
+      <c r="T14" s="22"/>
+      <c r="U14" s="22"/>
+      <c r="V14" s="22"/>
+      <c r="W14" s="22"/>
+      <c r="X14" s="22"/>
+      <c r="Y14" s="22"/>
+      <c r="Z14" s="25"/>
+      <c r="AA14" s="18"/>
+      <c r="AB14" s="25"/>
+      <c r="AC14" s="18"/>
+      <c r="AD14" s="25"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A15" s="49"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D15" s="20">
         <v>0.45</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E15" s="23">
         <v>0.45</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F15" s="23">
         <v>0.45</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G15" s="23">
         <v>0.45</v>
       </c>
-      <c r="H14" s="24">
+      <c r="H15" s="20">
+        <v>0.45</v>
+      </c>
+      <c r="I15" s="23">
         <v>0.46</v>
       </c>
-      <c r="I14" s="27">
+      <c r="J15" s="23">
         <v>0.45</v>
       </c>
-      <c r="J14" s="24"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="27"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="27"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="27"/>
-      <c r="U14" s="30"/>
-    </row>
-    <row r="15" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="52"/>
-      <c r="B15" s="54" t="s">
+      <c r="K15" s="20">
+        <v>0.44</v>
+      </c>
+      <c r="L15" s="23">
+        <v>0.43</v>
+      </c>
+      <c r="M15" s="23">
+        <v>0.43</v>
+      </c>
+      <c r="N15" s="23">
+        <v>0.49</v>
+      </c>
+      <c r="O15" s="23">
+        <v>0.44</v>
+      </c>
+      <c r="P15" s="23">
+        <v>0.43</v>
+      </c>
+      <c r="Q15" s="23">
+        <v>0.43</v>
+      </c>
+      <c r="R15" s="26">
+        <v>0.49</v>
+      </c>
+      <c r="S15" s="20"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="23"/>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="23"/>
+      <c r="Z15" s="26"/>
+      <c r="AA15" s="20"/>
+      <c r="AB15" s="26"/>
+      <c r="AC15" s="20"/>
+      <c r="AD15" s="26"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" s="49"/>
+      <c r="B16" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C16" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D16" s="16">
         <v>31.6</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E16" s="21">
         <v>31.6</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F16" s="21">
         <v>31.6</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G16" s="21">
         <v>31.7</v>
       </c>
-      <c r="H15" s="31"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="32"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="31"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="33"/>
-      <c r="S15" s="31"/>
-      <c r="T15" s="32"/>
-      <c r="U15" s="33"/>
-    </row>
-    <row r="16" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="21" t="s">
+      <c r="H16" s="27"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
+      <c r="W16" s="28"/>
+      <c r="X16" s="28"/>
+      <c r="Y16" s="28"/>
+      <c r="Z16" s="28"/>
+      <c r="AA16" s="28"/>
+      <c r="AB16" s="28"/>
+      <c r="AC16" s="28"/>
+      <c r="AD16" s="29"/>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A17" s="49"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D17" s="18">
         <v>47.3</v>
       </c>
-      <c r="E16" s="26">
+      <c r="E17" s="22">
         <v>47.3</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F17" s="22">
         <v>47.2</v>
       </c>
-      <c r="G16" s="26">
+      <c r="G17" s="22">
         <v>47.4</v>
       </c>
-      <c r="H16" s="34"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="36"/>
-      <c r="S16" s="34"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="36"/>
-    </row>
-    <row r="17" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="23" t="s">
+      <c r="H17" s="30"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="31"/>
+      <c r="R17" s="31"/>
+      <c r="S17" s="31"/>
+      <c r="T17" s="31"/>
+      <c r="U17" s="31"/>
+      <c r="V17" s="31"/>
+      <c r="W17" s="31"/>
+      <c r="X17" s="31"/>
+      <c r="Y17" s="31"/>
+      <c r="Z17" s="31"/>
+      <c r="AA17" s="31"/>
+      <c r="AB17" s="31"/>
+      <c r="AC17" s="31"/>
+      <c r="AD17" s="32"/>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A18" s="50"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D18" s="20">
         <v>0.45</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E18" s="23">
         <v>0.45</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F18" s="23">
         <v>0.45</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G18" s="23">
         <v>0.45</v>
       </c>
-      <c r="H17" s="37"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="38"/>
-      <c r="O17" s="38"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="38"/>
-      <c r="R17" s="39"/>
-      <c r="S17" s="37"/>
-      <c r="T17" s="38"/>
-      <c r="U17" s="39"/>
-    </row>
-    <row r="18" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="51" t="s">
+      <c r="H18" s="30"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="31"/>
+      <c r="R18" s="31"/>
+      <c r="S18" s="31"/>
+      <c r="T18" s="31"/>
+      <c r="U18" s="31"/>
+      <c r="V18" s="31"/>
+      <c r="W18" s="31"/>
+      <c r="X18" s="31"/>
+      <c r="Y18" s="31"/>
+      <c r="Z18" s="31"/>
+      <c r="AA18" s="31"/>
+      <c r="AB18" s="31"/>
+      <c r="AC18" s="31"/>
+      <c r="AD18" s="32"/>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="54" t="s">
+      <c r="B19" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C19" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D19" s="18">
         <v>29.9</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E19" s="22">
         <v>29.9</v>
       </c>
-      <c r="F18" s="43" t="s">
+      <c r="F19" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="26">
+      <c r="G19" s="22">
         <v>29.7</v>
       </c>
-      <c r="H18" s="34"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="36"/>
-      <c r="S18" s="34"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="36"/>
-    </row>
-    <row r="19" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="21" t="s">
+      <c r="H19" s="30"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="31"/>
+      <c r="R19" s="31"/>
+      <c r="S19" s="31"/>
+      <c r="T19" s="31"/>
+      <c r="U19" s="31"/>
+      <c r="V19" s="31"/>
+      <c r="W19" s="31"/>
+      <c r="X19" s="31"/>
+      <c r="Y19" s="31"/>
+      <c r="Z19" s="31"/>
+      <c r="AA19" s="31"/>
+      <c r="AB19" s="31"/>
+      <c r="AC19" s="31"/>
+      <c r="AD19" s="32"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A20" s="49"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D20" s="18">
         <v>50.4</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E20" s="22">
         <v>50.3</v>
       </c>
-      <c r="F19" s="43" t="s">
+      <c r="F20" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G20" s="22">
         <v>50.2</v>
       </c>
-      <c r="H19" s="34"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="34"/>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="36"/>
-      <c r="S19" s="34"/>
-      <c r="T19" s="35"/>
-      <c r="U19" s="36"/>
-    </row>
-    <row r="20" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="23" t="s">
+      <c r="H20" s="30"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
+      <c r="T20" s="31"/>
+      <c r="U20" s="31"/>
+      <c r="V20" s="31"/>
+      <c r="W20" s="31"/>
+      <c r="X20" s="31"/>
+      <c r="Y20" s="31"/>
+      <c r="Z20" s="31"/>
+      <c r="AA20" s="31"/>
+      <c r="AB20" s="31"/>
+      <c r="AC20" s="31"/>
+      <c r="AD20" s="32"/>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A21" s="50"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="24">
+      <c r="D21" s="20">
         <v>0.38</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E21" s="23">
         <v>0.38</v>
       </c>
-      <c r="F20" s="44" t="s">
+      <c r="F21" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G21" s="23">
         <v>0.38</v>
       </c>
-      <c r="H20" s="37"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="39"/>
-      <c r="S20" s="37"/>
-      <c r="T20" s="38"/>
-      <c r="U20" s="39"/>
-    </row>
-    <row r="21" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51" t="s">
+      <c r="H21" s="33"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="34"/>
+      <c r="T21" s="34"/>
+      <c r="U21" s="34"/>
+      <c r="V21" s="34"/>
+      <c r="W21" s="34"/>
+      <c r="X21" s="34"/>
+      <c r="Y21" s="34"/>
+      <c r="Z21" s="34"/>
+      <c r="AA21" s="34"/>
+      <c r="AB21" s="34"/>
+      <c r="AC21" s="34"/>
+      <c r="AD21" s="35"/>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="54" t="s">
+      <c r="B22" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C22" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D22" s="16">
         <v>33.1</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E22" s="21">
         <v>31.6</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F22" s="21">
         <v>32</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G22" s="21">
         <v>31.3</v>
       </c>
-      <c r="H21" s="20">
+      <c r="H22" s="16">
+        <v>33.1</v>
+      </c>
+      <c r="I22" s="21">
         <v>30.7</v>
       </c>
-      <c r="I21" s="25">
+      <c r="J22" s="21">
         <v>31.2</v>
       </c>
-      <c r="J21" s="20"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="28"/>
-      <c r="S21" s="20"/>
-      <c r="T21" s="25"/>
-      <c r="U21" s="28"/>
-    </row>
-    <row r="22" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="21" t="s">
+      <c r="K22" s="16">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="L22" s="21">
+        <v>44.8</v>
+      </c>
+      <c r="M22" s="21">
+        <v>39.6</v>
+      </c>
+      <c r="N22" s="21">
+        <v>23.3</v>
+      </c>
+      <c r="O22" s="21">
+        <v>61.7</v>
+      </c>
+      <c r="P22" s="21">
+        <v>43.3</v>
+      </c>
+      <c r="Q22" s="21">
+        <v>38.4</v>
+      </c>
+      <c r="R22" s="24">
+        <v>21.9</v>
+      </c>
+      <c r="S22" s="16"/>
+      <c r="T22" s="21"/>
+      <c r="U22" s="21"/>
+      <c r="V22" s="21"/>
+      <c r="W22" s="21"/>
+      <c r="X22" s="21"/>
+      <c r="Y22" s="21"/>
+      <c r="Z22" s="24"/>
+      <c r="AA22" s="16"/>
+      <c r="AB22" s="24"/>
+      <c r="AC22" s="16"/>
+      <c r="AD22" s="24"/>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A23" s="49"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D23" s="18">
         <v>48.8</v>
       </c>
-      <c r="E22" s="26">
+      <c r="E23" s="22">
         <v>47.4</v>
       </c>
-      <c r="F22" s="26">
+      <c r="F23" s="22">
         <v>48.4</v>
       </c>
-      <c r="G22" s="26">
+      <c r="G23" s="22">
         <v>47.3</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H23" s="18">
         <v>48.8</v>
       </c>
-      <c r="I22" s="26">
+      <c r="I23" s="22">
+        <v>48.8</v>
+      </c>
+      <c r="J23" s="22">
         <v>47.2</v>
       </c>
-      <c r="J22" s="22"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="29"/>
-      <c r="S22" s="22"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="29"/>
-    </row>
-    <row r="23" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="23" t="s">
+      <c r="K23" s="18">
+        <v>89</v>
+      </c>
+      <c r="L23" s="22">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="M23" s="22">
+        <v>60.1</v>
+      </c>
+      <c r="N23" s="22">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="O23" s="22">
+        <v>82.7</v>
+      </c>
+      <c r="P23" s="22">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="Q23" s="22">
+        <v>57.6</v>
+      </c>
+      <c r="R23" s="25">
+        <v>31.9</v>
+      </c>
+      <c r="S23" s="18"/>
+      <c r="T23" s="22"/>
+      <c r="U23" s="22"/>
+      <c r="V23" s="22"/>
+      <c r="W23" s="22"/>
+      <c r="X23" s="22"/>
+      <c r="Y23" s="22"/>
+      <c r="Z23" s="25"/>
+      <c r="AA23" s="18"/>
+      <c r="AB23" s="25"/>
+      <c r="AC23" s="18"/>
+      <c r="AD23" s="25"/>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A24" s="50"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D24" s="20">
         <v>0.41</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E24" s="23">
         <v>0.45</v>
       </c>
-      <c r="F23" s="27">
+      <c r="F24" s="23">
         <v>0.42</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G24" s="23">
         <v>0.45</v>
       </c>
-      <c r="H23" s="24">
+      <c r="H24" s="20">
         <v>0.41</v>
       </c>
-      <c r="I23" s="27">
+      <c r="I24" s="23">
+        <v>0.41</v>
+      </c>
+      <c r="J24" s="23">
         <v>0.45</v>
       </c>
-      <c r="J23" s="24"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="30"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="27"/>
-      <c r="R23" s="30"/>
-      <c r="S23" s="24"/>
-      <c r="T23" s="27"/>
-      <c r="U23" s="30"/>
-    </row>
-    <row r="24" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="51" t="s">
+      <c r="K24" s="20">
+        <v>0.33</v>
+      </c>
+      <c r="L24" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="M24" s="23">
+        <v>0.32</v>
+      </c>
+      <c r="N24" s="23">
+        <v>0.4</v>
+      </c>
+      <c r="O24" s="23">
+        <v>0.42</v>
+      </c>
+      <c r="P24" s="23">
+        <v>0.35</v>
+      </c>
+      <c r="Q24" s="23">
+        <v>0.37</v>
+      </c>
+      <c r="R24" s="26">
+        <v>0.42</v>
+      </c>
+      <c r="S24" s="20"/>
+      <c r="T24" s="23"/>
+      <c r="U24" s="23"/>
+      <c r="V24" s="23"/>
+      <c r="W24" s="23"/>
+      <c r="X24" s="23"/>
+      <c r="Y24" s="23"/>
+      <c r="Z24" s="26"/>
+      <c r="AA24" s="20"/>
+      <c r="AB24" s="26"/>
+      <c r="AC24" s="20"/>
+      <c r="AD24" s="26"/>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A25" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="54" t="s">
+      <c r="B25" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C25" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="20">
+      <c r="D25" s="16">
         <v>33.200000000000003</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E25" s="21">
         <v>31</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F25" s="21">
         <v>31.7</v>
       </c>
-      <c r="G24" s="40">
+      <c r="G25" s="36">
         <v>31.8</v>
       </c>
-      <c r="H24" s="20">
+      <c r="H25" s="16">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="I25" s="21">
         <v>31.3</v>
       </c>
-      <c r="I24" s="25">
+      <c r="J25" s="21">
         <v>31.2</v>
       </c>
-      <c r="J24" s="20"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="25"/>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="25"/>
-      <c r="R24" s="28"/>
-      <c r="S24" s="20"/>
-      <c r="T24" s="25"/>
-      <c r="U24" s="28"/>
-    </row>
-    <row r="25" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="52"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="21" t="s">
+      <c r="K25" s="16"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
+      <c r="V25" s="21"/>
+      <c r="W25" s="21"/>
+      <c r="X25" s="21"/>
+      <c r="Y25" s="21"/>
+      <c r="Z25" s="24"/>
+      <c r="AA25" s="16"/>
+      <c r="AB25" s="24"/>
+      <c r="AC25" s="16"/>
+      <c r="AD25" s="24"/>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A26" s="49"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D26" s="18">
         <v>49.3</v>
       </c>
-      <c r="E25" s="26">
+      <c r="E26" s="22">
         <v>47.1</v>
       </c>
-      <c r="F25" s="26">
+      <c r="F26" s="22">
         <v>47.4</v>
       </c>
-      <c r="G25" s="41">
+      <c r="G26" s="37">
         <v>47.1</v>
       </c>
-      <c r="H25" s="22">
+      <c r="H26" s="18">
+        <v>50.9</v>
+      </c>
+      <c r="I26" s="22">
         <v>46.7</v>
       </c>
-      <c r="I25" s="26">
+      <c r="J26" s="22">
         <v>46.7</v>
       </c>
-      <c r="J25" s="22"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="22"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="29"/>
-      <c r="S25" s="22"/>
-      <c r="T25" s="26"/>
-      <c r="U25" s="29"/>
-    </row>
-    <row r="26" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="53"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="23" t="s">
+      <c r="K26" s="18"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="25"/>
+      <c r="S26" s="18"/>
+      <c r="T26" s="22"/>
+      <c r="U26" s="22"/>
+      <c r="V26" s="22"/>
+      <c r="W26" s="22"/>
+      <c r="X26" s="22"/>
+      <c r="Y26" s="22"/>
+      <c r="Z26" s="25"/>
+      <c r="AA26" s="18"/>
+      <c r="AB26" s="25"/>
+      <c r="AC26" s="18"/>
+      <c r="AD26" s="25"/>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A27" s="50"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D27" s="20">
         <v>0.4</v>
       </c>
-      <c r="E26" s="27">
+      <c r="E27" s="23">
         <v>0.45</v>
       </c>
-      <c r="F26" s="27">
+      <c r="F27" s="23">
         <v>0.45</v>
       </c>
-      <c r="G26" s="42">
+      <c r="G27" s="38">
         <v>0.45</v>
       </c>
-      <c r="H26" s="24">
+      <c r="H27" s="20">
+        <v>0.36</v>
+      </c>
+      <c r="I27" s="23">
         <v>0.46</v>
       </c>
-      <c r="I26" s="27">
+      <c r="J27" s="23">
         <v>0.46</v>
       </c>
-      <c r="J26" s="24"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="27"/>
-      <c r="O26" s="27"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="27"/>
-      <c r="R26" s="30"/>
-      <c r="S26" s="24"/>
-      <c r="T26" s="27"/>
-      <c r="U26" s="30"/>
-    </row>
-    <row r="27" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="48" t="s">
+      <c r="K27" s="20"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="26"/>
+      <c r="S27" s="20"/>
+      <c r="T27" s="23"/>
+      <c r="U27" s="23"/>
+      <c r="V27" s="23"/>
+      <c r="W27" s="23"/>
+      <c r="X27" s="23"/>
+      <c r="Y27" s="23"/>
+      <c r="Z27" s="26"/>
+      <c r="AA27" s="20"/>
+      <c r="AB27" s="26"/>
+      <c r="AC27" s="20"/>
+      <c r="AD27" s="26"/>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A28" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="54" t="s">
+      <c r="B28" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C28" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="25"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="25"/>
-      <c r="R27" s="28"/>
-      <c r="S27" s="20"/>
-      <c r="T27" s="25"/>
-      <c r="U27" s="28"/>
-    </row>
-    <row r="28" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="49"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="21" t="s">
+      <c r="D28" s="16"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="21"/>
+      <c r="R28" s="24"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="21"/>
+      <c r="U28" s="21"/>
+      <c r="V28" s="21"/>
+      <c r="W28" s="21"/>
+      <c r="X28" s="21"/>
+      <c r="Y28" s="21"/>
+      <c r="Z28" s="24"/>
+      <c r="AA28" s="16"/>
+      <c r="AB28" s="24"/>
+      <c r="AC28" s="16"/>
+      <c r="AD28" s="24"/>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A29" s="46"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="26"/>
-      <c r="R28" s="29"/>
-      <c r="S28" s="22"/>
-      <c r="T28" s="26"/>
-      <c r="U28" s="29"/>
-    </row>
-    <row r="29" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="49"/>
-      <c r="B29" s="56"/>
-      <c r="C29" s="23" t="s">
+      <c r="D29" s="18"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="25"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="22"/>
+      <c r="U29" s="22"/>
+      <c r="V29" s="22"/>
+      <c r="W29" s="22"/>
+      <c r="X29" s="22"/>
+      <c r="Y29" s="22"/>
+      <c r="Z29" s="25"/>
+      <c r="AA29" s="18"/>
+      <c r="AB29" s="25"/>
+      <c r="AC29" s="18"/>
+      <c r="AD29" s="25"/>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A30" s="46"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="24"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="27"/>
-      <c r="R29" s="30"/>
-      <c r="S29" s="24"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="30"/>
-    </row>
-    <row r="30" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
-      <c r="B30" s="55" t="s">
+      <c r="D30" s="20"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="23"/>
+      <c r="R30" s="26"/>
+      <c r="S30" s="20"/>
+      <c r="T30" s="23"/>
+      <c r="U30" s="23"/>
+      <c r="V30" s="23"/>
+      <c r="W30" s="23"/>
+      <c r="X30" s="23"/>
+      <c r="Y30" s="23"/>
+      <c r="Z30" s="26"/>
+      <c r="AA30" s="20"/>
+      <c r="AB30" s="26"/>
+      <c r="AC30" s="20"/>
+      <c r="AD30" s="26"/>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A31" s="46"/>
+      <c r="B31" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C31" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="22"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="26"/>
-      <c r="O30" s="26"/>
-      <c r="P30" s="22"/>
-      <c r="Q30" s="26"/>
-      <c r="R30" s="29"/>
-      <c r="S30" s="22"/>
-      <c r="T30" s="26"/>
-      <c r="U30" s="29"/>
-    </row>
-    <row r="31" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="49"/>
-      <c r="B31" s="55"/>
-      <c r="C31" s="21" t="s">
+      <c r="D31" s="18"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="24"/>
+      <c r="S31" s="16"/>
+      <c r="T31" s="21"/>
+      <c r="U31" s="21"/>
+      <c r="V31" s="21"/>
+      <c r="W31" s="21"/>
+      <c r="X31" s="21"/>
+      <c r="Y31" s="21"/>
+      <c r="Z31" s="24"/>
+      <c r="AA31" s="18"/>
+      <c r="AB31" s="25"/>
+      <c r="AC31" s="18"/>
+      <c r="AD31" s="25"/>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A32" s="46"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="22"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="26"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="22"/>
-      <c r="Q31" s="26"/>
-      <c r="R31" s="29"/>
-      <c r="S31" s="22"/>
-      <c r="T31" s="26"/>
-      <c r="U31" s="29"/>
-    </row>
-    <row r="32" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
-      <c r="B32" s="56"/>
-      <c r="C32" s="23" t="s">
+      <c r="D32" s="18"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="22"/>
+      <c r="O32" s="22"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="25"/>
+      <c r="S32" s="18"/>
+      <c r="T32" s="22"/>
+      <c r="U32" s="22"/>
+      <c r="V32" s="22"/>
+      <c r="W32" s="22"/>
+      <c r="X32" s="22"/>
+      <c r="Y32" s="22"/>
+      <c r="Z32" s="25"/>
+      <c r="AA32" s="18"/>
+      <c r="AB32" s="25"/>
+      <c r="AC32" s="18"/>
+      <c r="AD32" s="25"/>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A33" s="47"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="24"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="24"/>
-      <c r="K32" s="27"/>
-      <c r="L32" s="30"/>
-      <c r="M32" s="24"/>
-      <c r="N32" s="27"/>
-      <c r="O32" s="27"/>
-      <c r="P32" s="24"/>
-      <c r="Q32" s="27"/>
-      <c r="R32" s="30"/>
-      <c r="S32" s="24"/>
-      <c r="T32" s="27"/>
-      <c r="U32" s="30"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="23"/>
+      <c r="R33" s="26"/>
+      <c r="S33" s="20"/>
+      <c r="T33" s="23"/>
+      <c r="U33" s="23"/>
+      <c r="V33" s="23"/>
+      <c r="W33" s="23"/>
+      <c r="X33" s="23"/>
+      <c r="Y33" s="23"/>
+      <c r="Z33" s="26"/>
+      <c r="AA33" s="20"/>
+      <c r="AB33" s="26"/>
+      <c r="AC33" s="20"/>
+      <c r="AD33" s="26"/>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A34" s="59"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3"/>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="3"/>
+      <c r="AC34" s="3"/>
+      <c r="AD34" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="A27:A32"/>
+  <mergeCells count="25">
+    <mergeCell ref="K1:R1"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="S1:Z1"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="A28:A33"/>
     <mergeCell ref="D1:G1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="A3:A17"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A4:A18"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3:XFD3 A6:XFD6 A9:XFD9 A12:XFD12 A18:XFD18 A15:XFD15 A21:XFD21 A24:XFD24 A27:XFD27 A30:XFD30">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="A4:H4 A7:H7 A10:H10 A13:H13 A19:H19 A16:H16 A22:H22 A25:H25 A28:R28 A31:R31 J25:R25 J22 J16:R16 J19:R19 J13:R13 J10:R10 J7:R7 J4:R4 AA4:XFD4 AA7:XFD7 AA10:XFD10 AA13:XFD13 AA19:XFD19 AA16:XFD16 AA22:XFD22 AA25:XFD25 AA31:XFD31 AA28:XFD28 O22:R22">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2418,7 +2995,187 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:XFD4 A7:XFD7 A10:XFD10 A13:XFD13 A16:XFD16 A19:XFD19 A22:XFD22 A25:XFD25 A28:XFD28 A31:XFD31">
+  <conditionalFormatting sqref="A5:H5 A8:H8 A11:H11 A14:H14 A17:H17 A20:H20 A23:H23 A26:H26 A29:R29 A32:R32 J26:R26 J23 J20:R20 J17:R17 J14:R14 J11:R11 J8:R8 J5:R5 AA5:XFD5 AA8:XFD8 AA11:XFD11 AA14:XFD14 AA17:XFD17 AA20:XFD20 AA23:XFD23 AA26:XFD26 AA32:XFD32 AA29:XFD29 O23:R23">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33:R33 A30:R30 A27:H27 A24:H24 A21:H21 A18:H18 A15:H15 A12:H12 A9:H9 A6:H6 J6:R6 J9:R9 J12:R12 J15:R15 J18:R18 J21:R21 J24 J27:R27 AA27:XFD27 AA24:XFD24 AA21:XFD21 AA18:XFD18 AA15:XFD15 AA12:XFD12 AA9:XFD9 AA6:XFD6 AA30:XFD30 AA33:XFD33 O24:R24">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7 I4 I10 I13 I19 I16 I22 I25">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8 I5 I11 I14 I17 I20 I23 I26">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24 I27 I21 I18 I15 I12 I9 I6">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S28:Z28 S31:Z31 S25:Z25 S16:Z16 S19:Z19 S13:Z13 S10:Z10 S7:Z7 S4:Z4">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S29:Z29 S32:Z32 S26:Z26 S20:Z20 S17:Z17 S14:Z14 S11:Z11 S8:Z8 S5:Z5">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S33:Z33 S30:Z30 S6:Z6 S9:Z9 S12:Z12 S15:Z15 S18:Z18 S21:Z21 S27:Z27">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K22:N22">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23:N23">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K24:N24">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W22:Z22">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W23:Z23">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W24:Z24">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S22:V22">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S23:V23">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2430,7 +3187,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A32:XFD32 A29:XFD29 A26:XFD26 A23:XFD23 A20:XFD20 A17:XFD17 A14:XFD14 A11:XFD11 A8:XFD8 A5:XFD5">
+  <conditionalFormatting sqref="S24:V24">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2453,7 +3210,7 @@
     <firstFooter>&amp;C_x000D__x000D__x000D_</firstFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="F18:F20" numberStoredAsText="1"/>
+    <ignoredError sqref="F20:F21" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
nn base model results
</commit_message>
<xml_diff>
--- a/modelIterations.xlsx
+++ b/modelIterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrkawa\Documents\Berkeley\w207\fantasyFootballML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A49F719-0617-41DF-9D95-C56C2590B9CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C519E5C2-ADEE-440A-AF7B-824039A888CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-4680" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1302,7 +1302,7 @@
   <dimension ref="A1:AD34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2596,10 +2596,18 @@
       <c r="J25" s="21">
         <v>31.2</v>
       </c>
-      <c r="K25" s="16"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
-      <c r="N25" s="21"/>
+      <c r="K25" s="16">
+        <v>62.9</v>
+      </c>
+      <c r="L25" s="21">
+        <v>46.2</v>
+      </c>
+      <c r="M25" s="21">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="N25" s="21">
+        <v>22.7</v>
+      </c>
       <c r="O25" s="21"/>
       <c r="P25" s="21"/>
       <c r="Q25" s="21"/>
@@ -2644,10 +2652,18 @@
       <c r="J26" s="22">
         <v>46.7</v>
       </c>
-      <c r="K26" s="18"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
+      <c r="K26" s="18">
+        <v>84.4</v>
+      </c>
+      <c r="L26" s="22">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="M26" s="22">
+        <v>58.3</v>
+      </c>
+      <c r="N26" s="22">
+        <v>32</v>
+      </c>
       <c r="O26" s="22"/>
       <c r="P26" s="22"/>
       <c r="Q26" s="22"/>
@@ -2692,10 +2708,18 @@
       <c r="J27" s="23">
         <v>0.46</v>
       </c>
-      <c r="K27" s="20"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
-      <c r="N27" s="23"/>
+      <c r="K27" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="L27" s="23">
+        <v>0.38</v>
+      </c>
+      <c r="M27" s="23">
+        <v>0.36</v>
+      </c>
+      <c r="N27" s="23">
+        <v>0.41</v>
+      </c>
       <c r="O27" s="23"/>
       <c r="P27" s="23"/>
       <c r="Q27" s="23"/>

</xml_diff>

<commit_message>
multioutput attempts; PCA refinement/NN results
</commit_message>
<xml_diff>
--- a/modelIterations.xlsx
+++ b/modelIterations.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrkawa\Documents\Berkeley\w207\fantasyFootballML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41117E93-2F2A-4F62-8158-D24FF429BB20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C179B6-3A17-4C78-98FE-A4D8D2113FC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8625" yWindow="-165" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modelIterations" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -155,7 +154,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,14 +296,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -487,12 +480,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5F5F5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -774,7 +761,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -961,12 +948,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1325,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W21" sqref="W21"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2030,14 +2011,30 @@
       <c r="R10" s="23">
         <v>20.9</v>
       </c>
-      <c r="S10" s="15"/>
-      <c r="T10" s="20"/>
-      <c r="U10" s="20"/>
-      <c r="V10" s="20"/>
-      <c r="W10" s="20"/>
-      <c r="X10" s="20"/>
-      <c r="Y10" s="20"/>
-      <c r="Z10" s="23"/>
+      <c r="S10" s="15">
+        <v>61.3</v>
+      </c>
+      <c r="T10" s="20">
+        <v>44.5</v>
+      </c>
+      <c r="U10" s="20">
+        <v>38.1</v>
+      </c>
+      <c r="V10" s="20">
+        <v>21.4</v>
+      </c>
+      <c r="W10" s="20">
+        <v>60.9</v>
+      </c>
+      <c r="X10" s="20">
+        <v>44.5</v>
+      </c>
+      <c r="Y10" s="20">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="Z10" s="23">
+        <v>21.1</v>
+      </c>
       <c r="AA10" s="15"/>
       <c r="AB10" s="20"/>
       <c r="AC10" s="20"/>
@@ -2114,14 +2111,30 @@
       <c r="R11" s="24">
         <v>29.7</v>
       </c>
-      <c r="S11" s="17"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="21"/>
-      <c r="X11" s="21"/>
-      <c r="Y11" s="21"/>
-      <c r="Z11" s="24"/>
+      <c r="S11" s="17">
+        <v>81</v>
+      </c>
+      <c r="T11" s="21">
+        <v>61.8</v>
+      </c>
+      <c r="U11" s="21">
+        <v>55.4</v>
+      </c>
+      <c r="V11" s="21">
+        <v>30.1</v>
+      </c>
+      <c r="W11" s="21">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="X11" s="21">
+        <v>61.9</v>
+      </c>
+      <c r="Y11" s="21">
+        <v>55.5</v>
+      </c>
+      <c r="Z11" s="24">
+        <v>30.1</v>
+      </c>
       <c r="AA11" s="17"/>
       <c r="AB11" s="21"/>
       <c r="AC11" s="21"/>
@@ -2198,14 +2211,30 @@
       <c r="R12" s="25">
         <v>0.49</v>
       </c>
-      <c r="S12" s="19"/>
-      <c r="T12" s="22"/>
-      <c r="U12" s="22"/>
-      <c r="V12" s="22"/>
-      <c r="W12" s="22"/>
-      <c r="X12" s="22"/>
-      <c r="Y12" s="22"/>
-      <c r="Z12" s="25"/>
+      <c r="S12" s="19">
+        <v>0.44</v>
+      </c>
+      <c r="T12" s="22">
+        <v>0.43</v>
+      </c>
+      <c r="U12" s="22">
+        <v>0.42</v>
+      </c>
+      <c r="V12" s="22">
+        <v>0.48</v>
+      </c>
+      <c r="W12" s="22">
+        <v>0.45</v>
+      </c>
+      <c r="X12" s="22">
+        <v>0.43</v>
+      </c>
+      <c r="Y12" s="22">
+        <v>0.42</v>
+      </c>
+      <c r="Z12" s="25">
+        <v>0.48</v>
+      </c>
       <c r="AA12" s="19"/>
       <c r="AB12" s="22"/>
       <c r="AC12" s="22"/>
@@ -2284,14 +2313,30 @@
       <c r="R13" s="24">
         <v>20.9</v>
       </c>
-      <c r="S13" s="17"/>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21"/>
-      <c r="W13" s="21"/>
-      <c r="X13" s="21"/>
-      <c r="Y13" s="21"/>
-      <c r="Z13" s="24"/>
+      <c r="S13" s="17">
+        <v>61.2</v>
+      </c>
+      <c r="T13" s="21">
+        <v>44.9</v>
+      </c>
+      <c r="U13" s="21">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="V13" s="21">
+        <v>21.6</v>
+      </c>
+      <c r="W13" s="21">
+        <v>61.2</v>
+      </c>
+      <c r="X13" s="21">
+        <v>44.4</v>
+      </c>
+      <c r="Y13" s="21">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="Z13" s="24">
+        <v>20.8</v>
+      </c>
       <c r="AA13" s="17"/>
       <c r="AB13" s="21"/>
       <c r="AC13" s="21"/>
@@ -2368,14 +2413,30 @@
       <c r="R14" s="24">
         <v>29.7</v>
       </c>
-      <c r="S14" s="17"/>
-      <c r="T14" s="21"/>
-      <c r="U14" s="21"/>
-      <c r="V14" s="21"/>
-      <c r="W14" s="21"/>
-      <c r="X14" s="21"/>
-      <c r="Y14" s="21"/>
-      <c r="Z14" s="24"/>
+      <c r="S14" s="17">
+        <v>80.8</v>
+      </c>
+      <c r="T14" s="21">
+        <v>62.1</v>
+      </c>
+      <c r="U14" s="21">
+        <v>55.3</v>
+      </c>
+      <c r="V14" s="21">
+        <v>30.1</v>
+      </c>
+      <c r="W14" s="21">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="X14" s="21">
+        <v>61.6</v>
+      </c>
+      <c r="Y14" s="21">
+        <v>55.3</v>
+      </c>
+      <c r="Z14" s="24">
+        <v>30.1</v>
+      </c>
       <c r="AA14" s="17"/>
       <c r="AB14" s="21"/>
       <c r="AC14" s="21"/>
@@ -2452,14 +2513,30 @@
       <c r="R15" s="25">
         <v>0.49</v>
       </c>
-      <c r="S15" s="19"/>
-      <c r="T15" s="22"/>
-      <c r="U15" s="22"/>
-      <c r="V15" s="22"/>
-      <c r="W15" s="22"/>
-      <c r="X15" s="22"/>
-      <c r="Y15" s="22"/>
-      <c r="Z15" s="25"/>
+      <c r="S15" s="19">
+        <v>0.45</v>
+      </c>
+      <c r="T15" s="22">
+        <v>0.42</v>
+      </c>
+      <c r="U15" s="22">
+        <v>0.42</v>
+      </c>
+      <c r="V15" s="22">
+        <v>0.48</v>
+      </c>
+      <c r="W15" s="22">
+        <v>0.45</v>
+      </c>
+      <c r="X15" s="22">
+        <v>0.43</v>
+      </c>
+      <c r="Y15" s="22">
+        <v>0.42</v>
+      </c>
+      <c r="Z15" s="25">
+        <v>0.48</v>
+      </c>
       <c r="AA15" s="19"/>
       <c r="AB15" s="22"/>
       <c r="AC15" s="22"/>
@@ -3222,14 +3299,30 @@
       <c r="R25" s="23">
         <v>22.5</v>
       </c>
-      <c r="S25" s="15"/>
-      <c r="T25" s="20"/>
-      <c r="U25" s="20"/>
-      <c r="V25" s="20"/>
-      <c r="W25" s="20"/>
-      <c r="X25" s="20"/>
-      <c r="Y25" s="20"/>
-      <c r="Z25" s="23"/>
+      <c r="S25" s="15">
+        <v>76</v>
+      </c>
+      <c r="T25" s="20">
+        <v>54.9</v>
+      </c>
+      <c r="U25" s="20">
+        <v>50.1</v>
+      </c>
+      <c r="V25" s="20">
+        <v>29.8</v>
+      </c>
+      <c r="W25" s="20">
+        <v>75</v>
+      </c>
+      <c r="X25" s="20">
+        <v>46.6</v>
+      </c>
+      <c r="Y25" s="20">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="Z25" s="23">
+        <v>21.7</v>
+      </c>
       <c r="AA25" s="15"/>
       <c r="AB25" s="20"/>
       <c r="AC25" s="20"/>
@@ -3306,14 +3399,30 @@
       <c r="R26" s="24">
         <v>32.6</v>
       </c>
-      <c r="S26" s="17"/>
-      <c r="T26" s="21"/>
-      <c r="U26" s="21"/>
-      <c r="V26" s="21"/>
-      <c r="W26" s="21"/>
-      <c r="X26" s="21"/>
-      <c r="Y26" s="21"/>
-      <c r="Z26" s="24"/>
+      <c r="S26" s="17">
+        <v>101.3</v>
+      </c>
+      <c r="T26" s="21">
+        <v>78.5</v>
+      </c>
+      <c r="U26" s="21">
+        <v>78.7</v>
+      </c>
+      <c r="V26" s="21">
+        <v>44.2</v>
+      </c>
+      <c r="W26" s="21">
+        <v>96</v>
+      </c>
+      <c r="X26" s="21">
+        <v>68.3</v>
+      </c>
+      <c r="Y26" s="21">
+        <v>59.1</v>
+      </c>
+      <c r="Z26" s="24">
+        <v>31.5</v>
+      </c>
       <c r="AA26" s="17"/>
       <c r="AB26" s="21"/>
       <c r="AC26" s="21"/>
@@ -3390,14 +3499,30 @@
       <c r="R27" s="25">
         <v>0.39</v>
       </c>
-      <c r="S27" s="19"/>
-      <c r="T27" s="22"/>
-      <c r="U27" s="22"/>
-      <c r="V27" s="22"/>
-      <c r="W27" s="22"/>
-      <c r="X27" s="22"/>
-      <c r="Y27" s="22"/>
-      <c r="Z27" s="25"/>
+      <c r="S27" s="19">
+        <v>0.13</v>
+      </c>
+      <c r="T27" s="22">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U27" s="22">
+        <v>-0.17</v>
+      </c>
+      <c r="V27" s="22">
+        <v>-0.12</v>
+      </c>
+      <c r="W27" s="22">
+        <v>0.22</v>
+      </c>
+      <c r="X27" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="Y27" s="22">
+        <v>0.34</v>
+      </c>
+      <c r="Z27" s="25">
+        <v>0.43</v>
+      </c>
       <c r="AA27" s="19"/>
       <c r="AB27" s="22"/>
       <c r="AC27" s="22"/>
@@ -4394,64 +4519,4 @@
     <ignoredError sqref="F20:F21" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D99E5869-D66F-4AC6-AC17-40299B9BBF6F}">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="A1:D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="63">
-        <v>63.4</v>
-      </c>
-      <c r="B1" s="63">
-        <v>44.1</v>
-      </c>
-      <c r="C1" s="63">
-        <v>38.200000000000003</v>
-      </c>
-      <c r="D1" s="63">
-        <v>22.7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="64">
-        <v>82.1</v>
-      </c>
-      <c r="B2" s="64">
-        <v>64.900000000000006</v>
-      </c>
-      <c r="C2" s="64">
-        <v>57.2</v>
-      </c>
-      <c r="D2" s="64">
-        <v>32.1</v>
-      </c>
-      <c r="E2" s="64"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="63">
-        <v>0.43</v>
-      </c>
-      <c r="B3" s="63">
-        <v>0.37</v>
-      </c>
-      <c r="C3" s="63">
-        <v>0.38</v>
-      </c>
-      <c r="D3" s="63">
-        <v>0.41</v>
-      </c>
-      <c r="E3" s="63"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
results through teammate data, except NN CV
</commit_message>
<xml_diff>
--- a/modelIterations.xlsx
+++ b/modelIterations.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrkawa\Documents\Berkeley\w207\fantasyFootballML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CB3C88-A317-4EC2-82F1-6385B53666DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BD7464-8426-4739-815F-1000FE155A37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modelIterations" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="40">
   <si>
     <t>Split by Position</t>
   </si>
@@ -154,7 +155,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,8 +297,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -480,6 +494,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -761,7 +781,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -934,6 +954,12 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -951,6 +977,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1309,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C3"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AU13" sqref="AU13:AX15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,9 +1428,9 @@
       <c r="AX1" s="46"/>
     </row>
     <row r="2" spans="1:50" s="1" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="58"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="60"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="62"/>
       <c r="D2" s="7" t="s">
         <v>30</v>
       </c>
@@ -1482,9 +1514,9 @@
       <c r="AX2" s="49"/>
     </row>
     <row r="3" spans="1:50" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="61"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="63"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="65"/>
       <c r="D3" s="36" t="s">
         <v>38</v>
       </c>
@@ -2534,10 +2566,18 @@
       <c r="AL13" s="16">
         <v>23.6</v>
       </c>
-      <c r="AM13" s="16"/>
-      <c r="AN13" s="16"/>
-      <c r="AO13" s="16"/>
-      <c r="AP13" s="19"/>
+      <c r="AM13" s="16">
+        <v>52.4</v>
+      </c>
+      <c r="AN13" s="16">
+        <v>39.9</v>
+      </c>
+      <c r="AO13" s="16">
+        <v>35.4</v>
+      </c>
+      <c r="AP13" s="19">
+        <v>23</v>
+      </c>
       <c r="AQ13" s="12">
         <v>53.2</v>
       </c>
@@ -2550,10 +2590,18 @@
       <c r="AT13" s="16">
         <v>22.7</v>
       </c>
-      <c r="AU13" s="16"/>
-      <c r="AV13" s="16"/>
-      <c r="AW13" s="16"/>
-      <c r="AX13" s="19"/>
+      <c r="AU13" s="16">
+        <v>52.9</v>
+      </c>
+      <c r="AV13" s="16">
+        <v>39.5</v>
+      </c>
+      <c r="AW13" s="16">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="AX13" s="19">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" s="56"/>
@@ -2666,10 +2714,18 @@
       <c r="AL14" s="16">
         <v>32.200000000000003</v>
       </c>
-      <c r="AM14" s="16"/>
-      <c r="AN14" s="16"/>
-      <c r="AO14" s="16"/>
-      <c r="AP14" s="19"/>
+      <c r="AM14" s="16">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="AN14" s="16">
+        <v>52.9</v>
+      </c>
+      <c r="AO14" s="16">
+        <v>49</v>
+      </c>
+      <c r="AP14" s="19">
+        <v>31.7</v>
+      </c>
       <c r="AQ14" s="12">
         <v>69</v>
       </c>
@@ -2682,10 +2738,18 @@
       <c r="AT14" s="16">
         <v>29.6</v>
       </c>
-      <c r="AU14" s="16"/>
-      <c r="AV14" s="16"/>
-      <c r="AW14" s="16"/>
-      <c r="AX14" s="19"/>
+      <c r="AU14" s="16">
+        <v>68.5</v>
+      </c>
+      <c r="AV14" s="16">
+        <v>54.9</v>
+      </c>
+      <c r="AW14" s="16">
+        <v>49.6</v>
+      </c>
+      <c r="AX14" s="19">
+        <v>29.2</v>
+      </c>
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" s="56"/>
@@ -2798,10 +2862,18 @@
       <c r="AL15" s="17">
         <v>0.45</v>
       </c>
-      <c r="AM15" s="17"/>
-      <c r="AN15" s="17"/>
-      <c r="AO15" s="17"/>
-      <c r="AP15" s="20"/>
+      <c r="AM15" s="17">
+        <v>0.48</v>
+      </c>
+      <c r="AN15" s="17">
+        <v>0.41</v>
+      </c>
+      <c r="AO15" s="17">
+        <v>0.37</v>
+      </c>
+      <c r="AP15" s="20">
+        <v>0.46</v>
+      </c>
       <c r="AQ15" s="14">
         <v>0.53</v>
       </c>
@@ -2814,10 +2886,18 @@
       <c r="AT15" s="17">
         <v>0.38</v>
       </c>
-      <c r="AU15" s="17"/>
-      <c r="AV15" s="17"/>
-      <c r="AW15" s="17"/>
-      <c r="AX15" s="20"/>
+      <c r="AU15" s="17">
+        <v>0.54</v>
+      </c>
+      <c r="AV15" s="17">
+        <v>0.43</v>
+      </c>
+      <c r="AW15" s="17">
+        <v>0.43</v>
+      </c>
+      <c r="AX15" s="20">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" s="56"/>
@@ -4945,4 +5025,70 @@
     <ignoredError sqref="F20:F21" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231F6EA-36D1-4E59-A8F8-5864590C36B9}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="59">
+        <v>52.9</v>
+      </c>
+      <c r="C1" s="59">
+        <v>39.5</v>
+      </c>
+      <c r="D1" s="59">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="E1" s="59">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="67">
+        <v>68.5</v>
+      </c>
+      <c r="C2" s="67">
+        <v>54.9</v>
+      </c>
+      <c r="D2" s="67">
+        <v>49.6</v>
+      </c>
+      <c r="E2" s="67">
+        <v>29.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="59">
+        <v>0.54</v>
+      </c>
+      <c r="C3" s="59">
+        <v>0.43</v>
+      </c>
+      <c r="D3" s="59">
+        <v>0.43</v>
+      </c>
+      <c r="E3" s="59">
+        <v>0.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
nn res for opponent and teammate data
</commit_message>
<xml_diff>
--- a/modelIterations.xlsx
+++ b/modelIterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrkawa\Documents\Berkeley\w207\fantasyFootballML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BD7464-8426-4739-815F-1000FE155A37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046ECFF8-6196-4769-9CDD-76E76F6BDF3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -311,7 +311,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -494,6 +494,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -954,6 +960,12 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -977,12 +989,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1341,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AU13" sqref="AU13:AX15"/>
+    <sheetView tabSelected="1" topLeftCell="N10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH28" sqref="AH28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,9 +1434,9 @@
       <c r="AX1" s="46"/>
     </row>
     <row r="2" spans="1:50" s="1" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="60"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="62"/>
+      <c r="A2" s="62"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="64"/>
       <c r="D2" s="7" t="s">
         <v>30</v>
       </c>
@@ -1514,9 +1520,9 @@
       <c r="AX2" s="49"/>
     </row>
     <row r="3" spans="1:50" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="63"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="65"/>
+      <c r="A3" s="65"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="67"/>
       <c r="D3" s="36" t="s">
         <v>38</v>
       </c>
@@ -3840,10 +3846,18 @@
       <c r="AL25" s="15">
         <v>24.3</v>
       </c>
-      <c r="AM25" s="15"/>
-      <c r="AN25" s="15"/>
-      <c r="AO25" s="15"/>
-      <c r="AP25" s="18"/>
+      <c r="AM25" s="15">
+        <v>53.2</v>
+      </c>
+      <c r="AN25" s="15">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="AO25" s="15">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="AP25" s="18">
+        <v>22.6</v>
+      </c>
       <c r="AQ25" s="10">
         <v>55.7</v>
       </c>
@@ -3856,10 +3870,18 @@
       <c r="AT25" s="15">
         <v>23.7</v>
       </c>
-      <c r="AU25" s="15"/>
-      <c r="AV25" s="15"/>
-      <c r="AW25" s="15"/>
-      <c r="AX25" s="18"/>
+      <c r="AU25" s="15">
+        <v>54.6</v>
+      </c>
+      <c r="AV25" s="15">
+        <v>40</v>
+      </c>
+      <c r="AW25" s="15">
+        <v>38.9</v>
+      </c>
+      <c r="AX25" s="18">
+        <v>23.1</v>
+      </c>
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A26" s="56"/>
@@ -3972,10 +3994,18 @@
       <c r="AL26" s="16">
         <v>33.200000000000003</v>
       </c>
-      <c r="AM26" s="16"/>
-      <c r="AN26" s="16"/>
-      <c r="AO26" s="16"/>
-      <c r="AP26" s="19"/>
+      <c r="AM26" s="16">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="AN26" s="16">
+        <v>54.5</v>
+      </c>
+      <c r="AO26" s="16">
+        <v>49.7</v>
+      </c>
+      <c r="AP26" s="19">
+        <v>31.9</v>
+      </c>
       <c r="AQ26" s="12">
         <v>75.400000000000006</v>
       </c>
@@ -3988,10 +4018,18 @@
       <c r="AT26" s="16">
         <v>31.3</v>
       </c>
-      <c r="AU26" s="16"/>
-      <c r="AV26" s="16"/>
-      <c r="AW26" s="16"/>
-      <c r="AX26" s="19"/>
+      <c r="AU26" s="16">
+        <v>69.8</v>
+      </c>
+      <c r="AV26" s="16">
+        <v>56.4</v>
+      </c>
+      <c r="AW26" s="16">
+        <v>52.4</v>
+      </c>
+      <c r="AX26" s="19">
+        <v>31.1</v>
+      </c>
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A27" s="57"/>
@@ -4104,10 +4142,18 @@
       <c r="AL27" s="17">
         <v>0.41</v>
       </c>
-      <c r="AM27" s="17"/>
-      <c r="AN27" s="17"/>
-      <c r="AO27" s="17"/>
-      <c r="AP27" s="20"/>
+      <c r="AM27" s="17">
+        <v>0.46</v>
+      </c>
+      <c r="AN27" s="17">
+        <v>0.37</v>
+      </c>
+      <c r="AO27" s="17">
+        <v>0.35</v>
+      </c>
+      <c r="AP27" s="20">
+        <v>0.45</v>
+      </c>
       <c r="AQ27" s="14">
         <v>0.44</v>
       </c>
@@ -4120,10 +4166,18 @@
       <c r="AT27" s="17">
         <v>0.31</v>
       </c>
-      <c r="AU27" s="17"/>
-      <c r="AV27" s="17"/>
-      <c r="AW27" s="17"/>
-      <c r="AX27" s="20"/>
+      <c r="AU27" s="17">
+        <v>0.52</v>
+      </c>
+      <c r="AV27" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="AW27" s="17">
+        <v>0.36</v>
+      </c>
+      <c r="AX27" s="20">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="28" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A28" s="52" t="s">
@@ -5031,9 +5085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231F6EA-36D1-4E59-A8F8-5864590C36B9}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5042,33 +5094,33 @@
         <v>24</v>
       </c>
       <c r="B1" s="59">
-        <v>52.9</v>
+        <v>54.6</v>
       </c>
       <c r="C1" s="59">
-        <v>39.5</v>
+        <v>40</v>
       </c>
       <c r="D1" s="59">
-        <v>36.700000000000003</v>
+        <v>38.9</v>
       </c>
       <c r="E1" s="59">
-        <v>22</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="67">
-        <v>68.5</v>
-      </c>
-      <c r="C2" s="67">
-        <v>54.9</v>
-      </c>
-      <c r="D2" s="67">
-        <v>49.6</v>
-      </c>
-      <c r="E2" s="67">
-        <v>29.2</v>
+      <c r="B2" s="61">
+        <v>69.8</v>
+      </c>
+      <c r="C2" s="61">
+        <v>56.4</v>
+      </c>
+      <c r="D2" s="61">
+        <v>52.4</v>
+      </c>
+      <c r="E2" s="61">
+        <v>31.1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -5076,16 +5128,16 @@
         <v>22</v>
       </c>
       <c r="B3" s="59">
-        <v>0.54</v>
+        <v>0.52</v>
       </c>
       <c r="C3" s="59">
-        <v>0.43</v>
+        <v>0.4</v>
       </c>
       <c r="D3" s="59">
-        <v>0.43</v>
+        <v>0.36</v>
       </c>
       <c r="E3" s="59">
-        <v>0.4</v>
+        <v>0.32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated results for decision trees
</commit_message>
<xml_diff>
--- a/modelIterations.xlsx
+++ b/modelIterations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrkawa\Documents\Berkeley\w207\fantasyFootballML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046ECFF8-6196-4769-9CDD-76E76F6BDF3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C572D48-609E-4033-8A54-12B2621D31C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modelIterations" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="39">
   <si>
     <t>Split by Position</t>
   </si>
@@ -77,12 +77,6 @@
   </si>
   <si>
     <t>MLP</t>
-  </si>
-  <si>
-    <t>Trees</t>
-  </si>
-  <si>
-    <t>Decision Tree</t>
   </si>
   <si>
     <t>Random Forest</t>
@@ -150,12 +144,15 @@
   <si>
     <t>Season Total + Game Mean Data</t>
   </si>
+  <si>
+    <t>Decision Trees</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,14 +295,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -510,7 +513,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -742,6 +745,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -918,6 +947,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -927,14 +971,20 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -942,36 +992,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -990,6 +1010,13 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1345,10 +1372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX34"/>
+  <dimension ref="A1:AX31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH28" sqref="AH28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,312 +1395,312 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="44" t="s">
+      <c r="A1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="44" t="s">
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="AB1" s="45"/>
-      <c r="AC1" s="45"/>
-      <c r="AD1" s="45"/>
-      <c r="AE1" s="45"/>
-      <c r="AF1" s="45"/>
-      <c r="AG1" s="45"/>
-      <c r="AH1" s="46"/>
-      <c r="AI1" s="44" t="s">
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50"/>
+      <c r="AE1" s="50"/>
+      <c r="AF1" s="50"/>
+      <c r="AG1" s="50"/>
+      <c r="AH1" s="51"/>
+      <c r="AI1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="AJ1" s="45"/>
-      <c r="AK1" s="45"/>
-      <c r="AL1" s="45"/>
-      <c r="AM1" s="45"/>
-      <c r="AN1" s="45"/>
-      <c r="AO1" s="45"/>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="44" t="s">
+      <c r="AJ1" s="50"/>
+      <c r="AK1" s="50"/>
+      <c r="AL1" s="50"/>
+      <c r="AM1" s="50"/>
+      <c r="AN1" s="50"/>
+      <c r="AO1" s="50"/>
+      <c r="AP1" s="51"/>
+      <c r="AQ1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="AR1" s="45"/>
-      <c r="AS1" s="45"/>
-      <c r="AT1" s="45"/>
-      <c r="AU1" s="45"/>
-      <c r="AV1" s="45"/>
-      <c r="AW1" s="45"/>
-      <c r="AX1" s="46"/>
+      <c r="AR1" s="50"/>
+      <c r="AS1" s="50"/>
+      <c r="AT1" s="50"/>
+      <c r="AU1" s="50"/>
+      <c r="AV1" s="50"/>
+      <c r="AW1" s="50"/>
+      <c r="AX1" s="51"/>
     </row>
     <row r="2" spans="1:50" s="1" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="64"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="61"/>
       <c r="D2" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
-      <c r="V2" s="48"/>
-      <c r="W2" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="49"/>
-      <c r="AA2" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB2" s="48"/>
-      <c r="AC2" s="48"/>
-      <c r="AD2" s="48"/>
-      <c r="AE2" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF2" s="48"/>
-      <c r="AG2" s="48"/>
-      <c r="AH2" s="49"/>
-      <c r="AI2" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="AJ2" s="48"/>
-      <c r="AK2" s="48"/>
-      <c r="AL2" s="48"/>
-      <c r="AM2" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN2" s="48"/>
-      <c r="AO2" s="48"/>
-      <c r="AP2" s="49"/>
-      <c r="AQ2" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="AR2" s="48"/>
-      <c r="AS2" s="48"/>
-      <c r="AT2" s="48"/>
-      <c r="AU2" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV2" s="48"/>
-      <c r="AW2" s="48"/>
-      <c r="AX2" s="49"/>
+      <c r="K2" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="47"/>
+      <c r="Z2" s="48"/>
+      <c r="AA2" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF2" s="47"/>
+      <c r="AG2" s="47"/>
+      <c r="AH2" s="48"/>
+      <c r="AI2" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ2" s="47"/>
+      <c r="AK2" s="47"/>
+      <c r="AL2" s="47"/>
+      <c r="AM2" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN2" s="47"/>
+      <c r="AO2" s="47"/>
+      <c r="AP2" s="48"/>
+      <c r="AQ2" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="AR2" s="47"/>
+      <c r="AS2" s="47"/>
+      <c r="AT2" s="47"/>
+      <c r="AU2" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="AV2" s="47"/>
+      <c r="AW2" s="47"/>
+      <c r="AX2" s="48"/>
     </row>
     <row r="3" spans="1:50" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="65"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="67"/>
+      <c r="A3" s="62"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="64"/>
       <c r="D3" s="36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G3" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I3" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J3" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K3" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="37" t="s">
+      <c r="N3" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="37" t="s">
-        <v>34</v>
-      </c>
       <c r="O3" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="37" t="s">
+      <c r="R3" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" s="37" t="s">
-        <v>34</v>
-      </c>
       <c r="S3" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="U3" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="T3" s="38" t="s">
+      <c r="V3" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="U3" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="V3" s="38" t="s">
-        <v>34</v>
-      </c>
       <c r="W3" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="X3" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y3" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="X3" s="38" t="s">
+      <c r="Z3" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="Y3" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z3" s="38" t="s">
-        <v>34</v>
-      </c>
       <c r="AA3" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB3" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC3" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="AB3" s="37" t="s">
+      <c r="AD3" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="AC3" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD3" s="37" t="s">
-        <v>34</v>
-      </c>
       <c r="AE3" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF3" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG3" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="AF3" s="37" t="s">
+      <c r="AH3" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="AG3" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="AH3" s="37" t="s">
-        <v>34</v>
-      </c>
       <c r="AI3" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ3" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK3" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="AJ3" s="38" t="s">
+      <c r="AL3" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="AK3" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL3" s="38" t="s">
-        <v>34</v>
-      </c>
       <c r="AM3" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN3" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="AO3" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="AN3" s="38" t="s">
+      <c r="AP3" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="AO3" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="AP3" s="38" t="s">
-        <v>34</v>
-      </c>
       <c r="AQ3" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="AR3" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="AS3" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="AR3" s="38" t="s">
+      <c r="AT3" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="AS3" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="AT3" s="38" t="s">
-        <v>34</v>
-      </c>
       <c r="AU3" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="AV3" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="AW3" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="AV3" s="38" t="s">
+      <c r="AX3" s="35" t="s">
         <v>32</v>
-      </c>
-      <c r="AW3" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="AX3" s="35" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="57" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="10">
         <v>31.7</v>
@@ -1726,10 +1753,10 @@
       <c r="AX4" s="23"/>
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A5" s="56"/>
-      <c r="B5" s="49"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="48"/>
       <c r="C5" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" s="12">
         <v>47.1</v>
@@ -1782,10 +1809,10 @@
       <c r="AX5" s="26"/>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A6" s="56"/>
-      <c r="B6" s="51"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" s="14">
         <v>0.45</v>
@@ -1838,12 +1865,12 @@
       <c r="AX6" s="26"/>
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
-      <c r="B7" s="50" t="s">
-        <v>20</v>
+      <c r="A7" s="55"/>
+      <c r="B7" s="57" t="s">
+        <v>18</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D7" s="10">
         <v>31.7</v>
@@ -1898,10 +1925,10 @@
       <c r="AX7" s="26"/>
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A8" s="56"/>
-      <c r="B8" s="49"/>
+      <c r="A8" s="55"/>
+      <c r="B8" s="48"/>
       <c r="C8" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="12">
         <v>47.4</v>
@@ -1956,10 +1983,10 @@
       <c r="AX8" s="26"/>
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A9" s="56"/>
-      <c r="B9" s="51"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" s="14">
         <v>0.45</v>
@@ -2014,12 +2041,12 @@
       <c r="AX9" s="29"/>
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
-      <c r="B10" s="50" t="s">
+      <c r="A10" s="55"/>
+      <c r="B10" s="57" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" s="10">
         <v>31.6</v>
@@ -2164,10 +2191,10 @@
       </c>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
-      <c r="B11" s="49"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D11" s="12">
         <v>47.3</v>
@@ -2312,10 +2339,10 @@
       </c>
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
-      <c r="B12" s="51"/>
+      <c r="A12" s="55"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12" s="14">
         <v>0.45</v>
@@ -2460,12 +2487,12 @@
       </c>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A13" s="56"/>
-      <c r="B13" s="50" t="s">
+      <c r="A13" s="55"/>
+      <c r="B13" s="57" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13" s="10">
         <v>31.6</v>
@@ -2610,10 +2637,10 @@
       </c>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A14" s="56"/>
-      <c r="B14" s="49"/>
+      <c r="A14" s="55"/>
+      <c r="B14" s="48"/>
       <c r="C14" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D14" s="12">
         <v>47.3</v>
@@ -2758,10 +2785,10 @@
       </c>
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A15" s="56"/>
-      <c r="B15" s="51"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="58"/>
       <c r="C15" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D15" s="14">
         <v>0.45</v>
@@ -2906,12 +2933,12 @@
       </c>
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A16" s="56"/>
-      <c r="B16" s="50" t="s">
+      <c r="A16" s="55"/>
+      <c r="B16" s="57" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D16" s="10">
         <v>31.6</v>
@@ -2970,10 +2997,10 @@
       <c r="AX16" s="23"/>
     </row>
     <row r="17" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A17" s="56"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="48"/>
       <c r="C17" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D17" s="12">
         <v>47.3</v>
@@ -3032,10 +3059,10 @@
       <c r="AX17" s="26"/>
     </row>
     <row r="18" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A18" s="57"/>
-      <c r="B18" s="51"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="58"/>
       <c r="C18" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D18" s="14">
         <v>0.45</v>
@@ -3094,14 +3121,14 @@
       <c r="AX18" s="26"/>
     </row>
     <row r="19" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="50" t="s">
-        <v>25</v>
+      <c r="B19" s="57" t="s">
+        <v>23</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D19" s="12">
         <v>29.9</v>
@@ -3110,7 +3137,7 @@
         <v>29.9</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G19" s="16">
         <v>29.7</v>
@@ -3160,10 +3187,10 @@
       <c r="AX19" s="26"/>
     </row>
     <row r="20" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A20" s="56"/>
-      <c r="B20" s="49"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="48"/>
       <c r="C20" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D20" s="12">
         <v>50.4</v>
@@ -3172,7 +3199,7 @@
         <v>50.3</v>
       </c>
       <c r="F20" s="33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G20" s="16">
         <v>50.2</v>
@@ -3222,10 +3249,10 @@
       <c r="AX20" s="26"/>
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A21" s="57"/>
-      <c r="B21" s="51"/>
+      <c r="A21" s="56"/>
+      <c r="B21" s="58"/>
       <c r="C21" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D21" s="14">
         <v>0.38</v>
@@ -3234,7 +3261,7 @@
         <v>0.38</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G21" s="17">
         <v>0.38</v>
@@ -3284,14 +3311,14 @@
       <c r="AX21" s="29"/>
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A22" s="55" t="s">
+      <c r="A22" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="50" t="s">
+      <c r="B22" s="57" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D22" s="10">
         <v>33.1</v>
@@ -3436,10 +3463,10 @@
       </c>
     </row>
     <row r="23" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A23" s="56"/>
-      <c r="B23" s="49"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="48"/>
       <c r="C23" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D23" s="12">
         <v>48.8</v>
@@ -3584,10 +3611,10 @@
       </c>
     </row>
     <row r="24" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A24" s="57"/>
-      <c r="B24" s="51"/>
+      <c r="A24" s="56"/>
+      <c r="B24" s="58"/>
       <c r="C24" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D24" s="14">
         <v>0.41</v>
@@ -3732,14 +3759,14 @@
       </c>
     </row>
     <row r="25" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A25" s="55" t="s">
+      <c r="A25" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D25" s="10">
         <v>33.200000000000003</v>
@@ -3884,10 +3911,10 @@
       </c>
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A26" s="56"/>
-      <c r="B26" s="49"/>
+      <c r="A26" s="55"/>
+      <c r="B26" s="48"/>
       <c r="C26" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D26" s="12">
         <v>49.3</v>
@@ -4032,10 +4059,10 @@
       </c>
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A27" s="57"/>
-      <c r="B27" s="51"/>
+      <c r="A27" s="56"/>
+      <c r="B27" s="58"/>
       <c r="C27" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D27" s="14">
         <v>0.4</v>
@@ -4181,29 +4208,49 @@
     </row>
     <row r="28" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A28" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="18"/>
+      <c r="C28" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="12">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16">
+        <v>37.9</v>
+      </c>
+      <c r="K28" s="10">
+        <v>66.2</v>
+      </c>
+      <c r="L28" s="15">
+        <v>42.8</v>
+      </c>
+      <c r="M28" s="15">
+        <v>35.5</v>
+      </c>
+      <c r="N28" s="15">
+        <v>23.8</v>
+      </c>
+      <c r="O28" s="15">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="P28" s="15">
+        <v>43.4</v>
+      </c>
+      <c r="Q28" s="15">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="R28" s="18">
+        <v>23</v>
+      </c>
       <c r="S28" s="10"/>
       <c r="T28" s="15"/>
       <c r="U28" s="15"/>
@@ -4212,52 +4259,120 @@
       <c r="X28" s="15"/>
       <c r="Y28" s="15"/>
       <c r="Z28" s="18"/>
-      <c r="AA28" s="10"/>
-      <c r="AB28" s="15"/>
-      <c r="AC28" s="15"/>
-      <c r="AD28" s="15"/>
-      <c r="AE28" s="15"/>
-      <c r="AF28" s="15"/>
-      <c r="AG28" s="15"/>
-      <c r="AH28" s="18"/>
-      <c r="AI28" s="10"/>
-      <c r="AJ28" s="15"/>
-      <c r="AK28" s="15"/>
-      <c r="AL28" s="15"/>
-      <c r="AM28" s="15"/>
-      <c r="AN28" s="15"/>
-      <c r="AO28" s="15"/>
-      <c r="AP28" s="18"/>
-      <c r="AQ28" s="10"/>
-      <c r="AR28" s="15"/>
-      <c r="AS28" s="15"/>
-      <c r="AT28" s="15"/>
-      <c r="AU28" s="15"/>
-      <c r="AV28" s="15"/>
-      <c r="AW28" s="15"/>
-      <c r="AX28" s="18"/>
+      <c r="AA28" s="10">
+        <v>60</v>
+      </c>
+      <c r="AB28" s="15">
+        <v>41.1</v>
+      </c>
+      <c r="AC28" s="15">
+        <v>36.9</v>
+      </c>
+      <c r="AD28" s="15">
+        <v>22.1</v>
+      </c>
+      <c r="AE28" s="15">
+        <v>61.4</v>
+      </c>
+      <c r="AF28" s="15">
+        <v>41.3</v>
+      </c>
+      <c r="AG28" s="15">
+        <v>37.1</v>
+      </c>
+      <c r="AH28" s="18">
+        <v>22.4</v>
+      </c>
+      <c r="AI28" s="10">
+        <v>51</v>
+      </c>
+      <c r="AJ28" s="15">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="AK28" s="15">
+        <v>33</v>
+      </c>
+      <c r="AL28" s="15">
+        <v>22.3</v>
+      </c>
+      <c r="AM28" s="15">
+        <v>51.2</v>
+      </c>
+      <c r="AN28" s="15">
+        <v>38.9</v>
+      </c>
+      <c r="AO28" s="15">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="AP28" s="18">
+        <v>22.6</v>
+      </c>
+      <c r="AQ28" s="10">
+        <v>50.7</v>
+      </c>
+      <c r="AR28" s="15">
+        <v>37.4</v>
+      </c>
+      <c r="AS28" s="15">
+        <v>35.9</v>
+      </c>
+      <c r="AT28" s="15">
+        <v>22.3</v>
+      </c>
+      <c r="AU28" s="15">
+        <v>50.5</v>
+      </c>
+      <c r="AV28" s="15">
+        <v>37.9</v>
+      </c>
+      <c r="AW28" s="15">
+        <v>35.9</v>
+      </c>
+      <c r="AX28" s="18">
+        <v>21.9</v>
+      </c>
     </row>
     <row r="29" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
-      <c r="B29" s="49"/>
+      <c r="A29" s="52"/>
+      <c r="B29" s="48"/>
       <c r="C29" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
-      <c r="H29" s="12"/>
+      <c r="H29" s="12">
+        <v>55</v>
+      </c>
       <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="19"/>
+      <c r="J29" s="16">
+        <v>55</v>
+      </c>
+      <c r="K29" s="12">
+        <v>81</v>
+      </c>
+      <c r="L29" s="16">
+        <v>62.8</v>
+      </c>
+      <c r="M29" s="16">
+        <v>52.9</v>
+      </c>
+      <c r="N29" s="16">
+        <v>32.5</v>
+      </c>
+      <c r="O29" s="16">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="P29" s="16">
+        <v>62.3</v>
+      </c>
+      <c r="Q29" s="16">
+        <v>53.4</v>
+      </c>
+      <c r="R29" s="19">
+        <v>31.6</v>
+      </c>
       <c r="S29" s="12"/>
       <c r="T29" s="16"/>
       <c r="U29" s="16"/>
@@ -4266,52 +4381,120 @@
       <c r="X29" s="16"/>
       <c r="Y29" s="16"/>
       <c r="Z29" s="19"/>
-      <c r="AA29" s="12"/>
-      <c r="AB29" s="16"/>
-      <c r="AC29" s="16"/>
-      <c r="AD29" s="16"/>
-      <c r="AE29" s="16"/>
-      <c r="AF29" s="16"/>
-      <c r="AG29" s="16"/>
-      <c r="AH29" s="19"/>
-      <c r="AI29" s="12"/>
-      <c r="AJ29" s="16"/>
-      <c r="AK29" s="16"/>
-      <c r="AL29" s="16"/>
-      <c r="AM29" s="16"/>
-      <c r="AN29" s="16"/>
-      <c r="AO29" s="16"/>
-      <c r="AP29" s="19"/>
-      <c r="AQ29" s="12"/>
-      <c r="AR29" s="16"/>
-      <c r="AS29" s="16"/>
-      <c r="AT29" s="16"/>
-      <c r="AU29" s="16"/>
-      <c r="AV29" s="16"/>
-      <c r="AW29" s="16"/>
-      <c r="AX29" s="19"/>
+      <c r="AA29" s="12">
+        <v>76</v>
+      </c>
+      <c r="AB29" s="16">
+        <v>63</v>
+      </c>
+      <c r="AC29" s="16">
+        <v>53.5</v>
+      </c>
+      <c r="AD29" s="16">
+        <v>30.3</v>
+      </c>
+      <c r="AE29" s="16">
+        <v>76.8</v>
+      </c>
+      <c r="AF29" s="16">
+        <v>63</v>
+      </c>
+      <c r="AG29" s="16">
+        <v>54.2</v>
+      </c>
+      <c r="AH29" s="19">
+        <v>30.7</v>
+      </c>
+      <c r="AI29" s="12">
+        <v>68.7</v>
+      </c>
+      <c r="AJ29" s="16">
+        <v>59.6</v>
+      </c>
+      <c r="AK29" s="16">
+        <v>48.5</v>
+      </c>
+      <c r="AL29" s="16">
+        <v>30.9</v>
+      </c>
+      <c r="AM29" s="16">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AN29" s="16">
+        <v>59.6</v>
+      </c>
+      <c r="AO29" s="16">
+        <v>48.6</v>
+      </c>
+      <c r="AP29" s="19">
+        <v>31.3</v>
+      </c>
+      <c r="AQ29" s="12">
+        <v>73.2</v>
+      </c>
+      <c r="AR29" s="16">
+        <v>59.6</v>
+      </c>
+      <c r="AS29" s="16">
+        <v>50.1</v>
+      </c>
+      <c r="AT29" s="16">
+        <v>30.3</v>
+      </c>
+      <c r="AU29" s="16">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="AV29" s="16">
+        <v>59.9</v>
+      </c>
+      <c r="AW29" s="16">
+        <v>50.6</v>
+      </c>
+      <c r="AX29" s="19">
+        <v>30.2</v>
+      </c>
     </row>
     <row r="30" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A30" s="53"/>
-      <c r="B30" s="51"/>
+      <c r="B30" s="58"/>
       <c r="C30" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D30" s="14"/>
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>
-      <c r="H30" s="14"/>
+      <c r="H30" s="14">
+        <v>0.47</v>
+      </c>
       <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17"/>
-      <c r="Q30" s="17"/>
-      <c r="R30" s="20"/>
+      <c r="J30" s="17">
+        <v>0.47</v>
+      </c>
+      <c r="K30" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="L30" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="M30" s="17">
+        <v>0.45</v>
+      </c>
+      <c r="N30" s="17">
+        <v>0.37</v>
+      </c>
+      <c r="O30" s="17">
+        <v>0.32</v>
+      </c>
+      <c r="P30" s="17">
+        <v>0.41</v>
+      </c>
+      <c r="Q30" s="17">
+        <v>0.44</v>
+      </c>
+      <c r="R30" s="20">
+        <v>0.41</v>
+      </c>
       <c r="S30" s="14"/>
       <c r="T30" s="17"/>
       <c r="U30" s="17"/>
@@ -4320,256 +4503,144 @@
       <c r="X30" s="17"/>
       <c r="Y30" s="17"/>
       <c r="Z30" s="20"/>
-      <c r="AA30" s="14"/>
-      <c r="AB30" s="17"/>
-      <c r="AC30" s="17"/>
-      <c r="AD30" s="17"/>
-      <c r="AE30" s="17"/>
-      <c r="AF30" s="17"/>
-      <c r="AG30" s="17"/>
-      <c r="AH30" s="20"/>
-      <c r="AI30" s="14"/>
-      <c r="AJ30" s="17"/>
-      <c r="AK30" s="17"/>
-      <c r="AL30" s="17"/>
-      <c r="AM30" s="17"/>
-      <c r="AN30" s="17"/>
-      <c r="AO30" s="17"/>
-      <c r="AP30" s="20"/>
-      <c r="AQ30" s="14"/>
-      <c r="AR30" s="17"/>
-      <c r="AS30" s="17"/>
-      <c r="AT30" s="17"/>
-      <c r="AU30" s="17"/>
-      <c r="AV30" s="17"/>
-      <c r="AW30" s="17"/>
-      <c r="AX30" s="20"/>
+      <c r="AA30" s="14">
+        <v>0.38</v>
+      </c>
+      <c r="AB30" s="17">
+        <v>0.39</v>
+      </c>
+      <c r="AC30" s="17">
+        <v>0.44</v>
+      </c>
+      <c r="AD30" s="17">
+        <v>0.45</v>
+      </c>
+      <c r="AE30" s="17">
+        <v>0.37</v>
+      </c>
+      <c r="AF30" s="17">
+        <v>0.39</v>
+      </c>
+      <c r="AG30" s="17">
+        <v>0.42</v>
+      </c>
+      <c r="AH30" s="20">
+        <v>0.44</v>
+      </c>
+      <c r="AI30" s="14">
+        <v>0.48</v>
+      </c>
+      <c r="AJ30" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="AK30" s="17">
+        <v>0.38</v>
+      </c>
+      <c r="AL30" s="17">
+        <v>0.49</v>
+      </c>
+      <c r="AM30" s="17">
+        <v>0.47</v>
+      </c>
+      <c r="AN30" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="AO30" s="17">
+        <v>0.38</v>
+      </c>
+      <c r="AP30" s="20">
+        <v>0.48</v>
+      </c>
+      <c r="AQ30" s="14">
+        <v>0.48</v>
+      </c>
+      <c r="AR30" s="17">
+        <v>0.33</v>
+      </c>
+      <c r="AS30" s="17">
+        <v>0.42</v>
+      </c>
+      <c r="AT30" s="17">
+        <v>0.35</v>
+      </c>
+      <c r="AU30" s="17">
+        <v>0.49</v>
+      </c>
+      <c r="AV30" s="17">
+        <v>0.32</v>
+      </c>
+      <c r="AW30" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="AX30" s="20">
+        <v>0.36</v>
+      </c>
     </row>
     <row r="31" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A31" s="53"/>
-      <c r="B31" s="49" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="10"/>
-      <c r="T31" s="15"/>
-      <c r="U31" s="15"/>
-      <c r="V31" s="15"/>
-      <c r="W31" s="15"/>
-      <c r="X31" s="15"/>
-      <c r="Y31" s="15"/>
-      <c r="Z31" s="18"/>
-      <c r="AA31" s="10"/>
-      <c r="AB31" s="15"/>
-      <c r="AC31" s="15"/>
-      <c r="AD31" s="15"/>
-      <c r="AE31" s="15"/>
-      <c r="AF31" s="15"/>
-      <c r="AG31" s="15"/>
-      <c r="AH31" s="18"/>
-      <c r="AI31" s="10"/>
-      <c r="AJ31" s="15"/>
-      <c r="AK31" s="15"/>
-      <c r="AL31" s="15"/>
-      <c r="AM31" s="15"/>
-      <c r="AN31" s="15"/>
-      <c r="AO31" s="15"/>
-      <c r="AP31" s="18"/>
-      <c r="AQ31" s="10"/>
-      <c r="AR31" s="15"/>
-      <c r="AS31" s="15"/>
-      <c r="AT31" s="15"/>
-      <c r="AU31" s="15"/>
-      <c r="AV31" s="15"/>
-      <c r="AW31" s="15"/>
-      <c r="AX31" s="18"/>
-    </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
-      <c r="B32" s="49"/>
-      <c r="C32" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="12"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
-      <c r="O32" s="16"/>
-      <c r="P32" s="16"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="19"/>
-      <c r="S32" s="12"/>
-      <c r="T32" s="16"/>
-      <c r="U32" s="16"/>
-      <c r="V32" s="16"/>
-      <c r="W32" s="16"/>
-      <c r="X32" s="16"/>
-      <c r="Y32" s="16"/>
-      <c r="Z32" s="19"/>
-      <c r="AA32" s="12"/>
-      <c r="AB32" s="16"/>
-      <c r="AC32" s="16"/>
-      <c r="AD32" s="16"/>
-      <c r="AE32" s="16"/>
-      <c r="AF32" s="16"/>
-      <c r="AG32" s="16"/>
-      <c r="AH32" s="19"/>
-      <c r="AI32" s="12"/>
-      <c r="AJ32" s="16"/>
-      <c r="AK32" s="16"/>
-      <c r="AL32" s="16"/>
-      <c r="AM32" s="16"/>
-      <c r="AN32" s="16"/>
-      <c r="AO32" s="16"/>
-      <c r="AP32" s="19"/>
-      <c r="AQ32" s="12"/>
-      <c r="AR32" s="16"/>
-      <c r="AS32" s="16"/>
-      <c r="AT32" s="16"/>
-      <c r="AU32" s="16"/>
-      <c r="AV32" s="16"/>
-      <c r="AW32" s="16"/>
-      <c r="AX32" s="19"/>
-    </row>
-    <row r="33" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A33" s="54"/>
-      <c r="B33" s="51"/>
-      <c r="C33" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="17"/>
-      <c r="M33" s="17"/>
-      <c r="N33" s="17"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="17"/>
-      <c r="Q33" s="17"/>
-      <c r="R33" s="20"/>
-      <c r="S33" s="14"/>
-      <c r="T33" s="17"/>
-      <c r="U33" s="17"/>
-      <c r="V33" s="17"/>
-      <c r="W33" s="17"/>
-      <c r="X33" s="17"/>
-      <c r="Y33" s="17"/>
-      <c r="Z33" s="20"/>
-      <c r="AA33" s="14"/>
-      <c r="AB33" s="17"/>
-      <c r="AC33" s="17"/>
-      <c r="AD33" s="17"/>
-      <c r="AE33" s="17"/>
-      <c r="AF33" s="17"/>
-      <c r="AG33" s="17"/>
-      <c r="AH33" s="20"/>
-      <c r="AI33" s="14"/>
-      <c r="AJ33" s="17"/>
-      <c r="AK33" s="17"/>
-      <c r="AL33" s="17"/>
-      <c r="AM33" s="17"/>
-      <c r="AN33" s="17"/>
-      <c r="AO33" s="17"/>
-      <c r="AP33" s="20"/>
-      <c r="AQ33" s="14"/>
-      <c r="AR33" s="17"/>
-      <c r="AS33" s="17"/>
-      <c r="AT33" s="17"/>
-      <c r="AU33" s="17"/>
-      <c r="AV33" s="17"/>
-      <c r="AW33" s="17"/>
-      <c r="AX33" s="20"/>
-    </row>
-    <row r="34" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A34" s="41"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
-      <c r="R34" s="3"/>
-      <c r="S34" s="3"/>
-      <c r="T34" s="3"/>
-      <c r="U34" s="3"/>
-      <c r="V34" s="3"/>
-      <c r="W34" s="3"/>
-      <c r="X34" s="3"/>
-      <c r="Y34" s="3"/>
-      <c r="Z34" s="3"/>
-      <c r="AA34" s="3"/>
-      <c r="AB34" s="3"/>
-      <c r="AC34" s="3"/>
-      <c r="AD34" s="3"/>
-      <c r="AE34" s="3"/>
-      <c r="AF34" s="3"/>
-      <c r="AG34" s="3"/>
-      <c r="AH34" s="3"/>
-      <c r="AI34" s="3"/>
-      <c r="AJ34" s="3"/>
-      <c r="AK34" s="3"/>
-      <c r="AL34" s="3"/>
-      <c r="AM34" s="3"/>
-      <c r="AN34" s="3"/>
-      <c r="AO34" s="3"/>
-      <c r="AP34" s="3"/>
-      <c r="AQ34" s="3"/>
-      <c r="AR34" s="3"/>
-      <c r="AS34" s="3"/>
-      <c r="AT34" s="3"/>
-      <c r="AU34" s="3"/>
-      <c r="AV34" s="3"/>
-      <c r="AW34" s="3"/>
-      <c r="AX34" s="3"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="3"/>
+      <c r="AC31" s="3"/>
+      <c r="AD31" s="3"/>
+      <c r="AE31" s="3"/>
+      <c r="AF31" s="3"/>
+      <c r="AG31" s="3"/>
+      <c r="AH31" s="3"/>
+      <c r="AI31" s="3"/>
+      <c r="AJ31" s="3"/>
+      <c r="AK31" s="3"/>
+      <c r="AL31" s="3"/>
+      <c r="AM31" s="3"/>
+      <c r="AN31" s="3"/>
+      <c r="AO31" s="3"/>
+      <c r="AP31" s="3"/>
+      <c r="AQ31" s="3"/>
+      <c r="AR31" s="3"/>
+      <c r="AS31" s="3"/>
+      <c r="AT31" s="3"/>
+      <c r="AU31" s="3"/>
+      <c r="AV31" s="3"/>
+      <c r="AW31" s="3"/>
+      <c r="AX31" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AI1:AP1"/>
-    <mergeCell ref="AQ1:AX1"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AU2:AX2"/>
-    <mergeCell ref="A28:A33"/>
+  <mergeCells count="32">
+    <mergeCell ref="AA1:AH1"/>
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="S1:Z1"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="K1:R1"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="A28:A30"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="H1:J1"/>
@@ -4585,20 +4656,15 @@
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A1:C3"/>
     <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="K1:R1"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="AA1:AH1"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="S1:Z1"/>
-    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AI1:AP1"/>
+    <mergeCell ref="AQ1:AX1"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="AU2:AX2"/>
   </mergeCells>
-  <conditionalFormatting sqref="AY4:XFD4 A4:H4 A7:H7 A10:H10 A13:H13 A19:H19 A16:H16 A22:H22 A25:H25 A28:R28 A31:R31 J25:R25 J22 J16:R16 J19:R19 J13:R13 J10:R10 J7:R7 J4:R4 AY7:XFD7 AY10:XFD10 AY13:XFD13 AY19:XFD19 AY16:XFD16 AY22:XFD22 AY25:XFD25 AY31:XFD31 AY28:XFD28 O22:R22">
-    <cfRule type="colorScale" priority="52">
+  <conditionalFormatting sqref="A28:G28 AY4:XFD4 A4:H4 A7:H7 A10:H10 A13:H13 A19:H19 A16:H16 A22:H22 A25:H25 J25:R25 J22 J16:R16 J19:R19 J13:R13 J10:R10 J7:R7 J4:R4 AY7:XFD7 AY10:XFD10 AY13:XFD13 AY19:XFD19 AY16:XFD16 AY22:XFD22 AY25:XFD25 AY28:XFD28 O22:R22 K28:R28">
+    <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4609,7 +4675,79 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AY5:XFD5 A5:H5 A8:H8 A11:H11 A14:H14 A17:H17 A20:H20 A23:H23 A26:H26 A29:R29 A32:R32 J26:R26 J23 J20:R20 J17:R17 J14:R14 J11:R11 J8:R8 J5:R5 AY8:XFD8 AY11:XFD11 AY14:XFD14 AY17:XFD17 AY20:XFD20 AY23:XFD23 AY26:XFD26 AY32:XFD32 AY29:XFD29 O23:R23">
+  <conditionalFormatting sqref="A29:G29 AY5:XFD5 A5:H5 A8:H8 A11:H11 A14:H14 A17:H17 A20:H20 A23:H23 A26:H26 J26:R26 J23 J20:R20 J17:R17 J14:R14 J11:R11 J8:R8 J5:R5 AY8:XFD8 AY11:XFD11 AY14:XFD14 AY17:XFD17 AY20:XFD20 AY23:XFD23 AY26:XFD26 AY29:XFD29 O23:R23 K29:R29">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30:G30 AY27:XFD27 A27:H27 A24:H24 A21:H21 A18:H18 A15:H15 A12:H12 A9:H9 A6:H6 J6:R6 J9:R9 J12:R12 J15:R15 J18:R18 J21:R21 J24 J27:R27 AY24:XFD24 AY21:XFD21 AY18:XFD18 AY15:XFD15 AY12:XFD12 AY9:XFD9 AY6:XFD6 AY30:XFD30 O24:R24 K30:R30">
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4 I7 I10 I13 I19 I16 I22 I25">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5 I8 I11 I14 I17 I20 I23 I26">
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27 I24 I21 I18 I15 I12 I9 I6">
+    <cfRule type="colorScale" priority="52">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA28:AH28 AA25:AH25 AA16:AH16 AA19:AH19 AA13:AH13 AA10:AH10 AA7:AH7 AA4:AH4">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA29:AH29 AA26:AH26 AA20:AH20 AA17:AH17 AA14:AH14 AA11:AH11 AA8:AH8 AA5:AH5">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
@@ -4621,7 +4759,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AY27:XFD27 A33:R33 A30:R30 A27:H27 A24:H24 A21:H21 A18:H18 A15:H15 A12:H12 A9:H9 A6:H6 J6:R6 J9:R9 J12:R12 J15:R15 J18:R18 J21:R21 J24 J27:R27 AY24:XFD24 AY21:XFD21 AY18:XFD18 AY15:XFD15 AY12:XFD12 AY9:XFD9 AY6:XFD6 AY30:XFD30 AY33:XFD33 O24:R24">
+  <conditionalFormatting sqref="AA30:AH30 AA6:AH6 AA9:AH9 AA12:AH12 AA15:AH15 AA18:AH18 AA21:AH21 AA27:AH27">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -4633,7 +4771,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4 I7 I10 I13 I19 I16 I22 I25">
+  <conditionalFormatting sqref="K22:N22">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
@@ -4645,7 +4783,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5 I8 I11 I14 I17 I20 I23 I26">
+  <conditionalFormatting sqref="K23:N23">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -4657,7 +4795,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I27 I24 I21 I18 I15 I12 I9 I6">
+  <conditionalFormatting sqref="K24:N24">
     <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
@@ -4669,8 +4807,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA28:AH28 AA31:AH31 AA25:AH25 AA16:AH16 AA19:AH19 AA13:AH13 AA10:AH10 AA7:AH7 AA4:AH4">
-    <cfRule type="colorScale" priority="45">
+  <conditionalFormatting sqref="S28:Z28 S25:Z25 S16:Z16 S19:Z19 S13:Z13 S10:Z10 S7:Z7 S4:Z4">
+    <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4681,8 +4819,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA29:AH29 AA32:AH32 AA26:AH26 AA20:AH20 AA17:AH17 AA14:AH14 AA11:AH11 AA8:AH8 AA5:AH5">
-    <cfRule type="colorScale" priority="44">
+  <conditionalFormatting sqref="S29:Z29 S26:Z26 S20:Z20 S17:Z17 S14:Z14 S11:Z11 S8:Z8 S5:Z5">
+    <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4693,8 +4831,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA33:AH33 AA30:AH30 AA6:AH6 AA9:AH9 AA12:AH12 AA15:AH15 AA18:AH18 AA21:AH21 AA27:AH27">
-    <cfRule type="colorScale" priority="43">
+  <conditionalFormatting sqref="S30:Z30 S6:Z6 S9:Z9 S12:Z12 S15:Z15 S18:Z18 S21:Z21 S27:Z27">
+    <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4705,8 +4843,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K22:N22">
-    <cfRule type="colorScale" priority="42">
+  <conditionalFormatting sqref="W22:Z22">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4717,8 +4855,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K23:N23">
-    <cfRule type="colorScale" priority="41">
+  <conditionalFormatting sqref="W23:Z23">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4729,8 +4867,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K24:N24">
-    <cfRule type="colorScale" priority="40">
+  <conditionalFormatting sqref="W24:Z24">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4741,7 +4879,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S28:Z28 S31:Z31 S25:Z25 S16:Z16 S19:Z19 S13:Z13 S10:Z10 S7:Z7 S4:Z4">
+  <conditionalFormatting sqref="S22:V22">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
@@ -4753,7 +4891,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S29:Z29 S32:Z32 S26:Z26 S20:Z20 S17:Z17 S14:Z14 S11:Z11 S8:Z8 S5:Z5">
+  <conditionalFormatting sqref="S23:V23">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -4765,7 +4903,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S33:Z33 S30:Z30 S6:Z6 S9:Z9 S12:Z12 S15:Z15 S18:Z18 S21:Z21 S27:Z27">
+  <conditionalFormatting sqref="S24:V24">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -4777,7 +4915,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W22:Z22">
+  <conditionalFormatting sqref="AQ28:AX28 AQ25:AX25 AQ16:AX16 AQ19:AX19 AQ13:AX13 AQ10:AX10 AQ7:AX7 AQ4:AX4">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -4789,7 +4927,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W23:Z23">
+  <conditionalFormatting sqref="AQ29:AX29 AQ26:AX26 AQ20:AX20 AQ17:AX17 AQ14:AX14 AQ11:AX11 AQ8:AX8 AQ5:AX5">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -4801,7 +4939,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W24:Z24">
+  <conditionalFormatting sqref="AQ30:AX30 AQ6:AX6 AQ9:AX9 AQ12:AX12 AQ15:AX15 AQ18:AX18 AQ21:AX21 AQ27:AX27">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -4813,7 +4951,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S22:V22">
+  <conditionalFormatting sqref="AU22:AX22">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -4825,7 +4963,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S23:V23">
+  <conditionalFormatting sqref="AU23:AX23">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -4837,7 +4975,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S24:V24">
+  <conditionalFormatting sqref="AU24:AX24">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -4849,7 +4987,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ28:AX28 AQ31:AX31 AQ25:AX25 AQ16:AX16 AQ19:AX19 AQ13:AX13 AQ10:AX10 AQ7:AX7 AQ4:AX4">
+  <conditionalFormatting sqref="AQ22:AT22">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -4861,7 +4999,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ29:AX29 AQ32:AX32 AQ26:AX26 AQ20:AX20 AQ17:AX17 AQ14:AX14 AQ11:AX11 AQ8:AX8 AQ5:AX5">
+  <conditionalFormatting sqref="AQ23:AT23">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -4873,7 +5011,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ33:AX33 AQ30:AX30 AQ6:AX6 AQ9:AX9 AQ12:AX12 AQ15:AX15 AQ18:AX18 AQ21:AX21 AQ27:AX27">
+  <conditionalFormatting sqref="AQ24:AT24">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -4885,7 +5023,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AU22:AX22">
+  <conditionalFormatting sqref="AI28:AP28 AI25:AP25 AI16:AP16 AI19:AP19 AI13:AP13 AI10:AP10 AI7:AP7 AI4:AP4">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -4897,7 +5035,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AU23:AX23">
+  <conditionalFormatting sqref="AI29:AP29 AI26:AP26 AI20:AP20 AI17:AP17 AI14:AP14 AI11:AP11 AI8:AP8 AI5:AP5">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -4909,7 +5047,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AU24:AX24">
+  <conditionalFormatting sqref="AI30:AP30 AI6:AP6 AI9:AP9 AI12:AP12 AI15:AP15 AI18:AP18 AI21:AP21 AI27:AP27">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -4921,8 +5059,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ22:AT22">
-    <cfRule type="colorScale" priority="18">
+  <conditionalFormatting sqref="AA22:AH22">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4933,8 +5071,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ23:AT23">
-    <cfRule type="colorScale" priority="17">
+  <conditionalFormatting sqref="AA23:AH23">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4945,8 +5083,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ24:AT24">
-    <cfRule type="colorScale" priority="16">
+  <conditionalFormatting sqref="AA24:AH24">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4957,8 +5095,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI28:AP28 AI31:AP31 AI25:AP25 AI16:AP16 AI19:AP19 AI13:AP13 AI10:AP10 AI7:AP7 AI4:AP4">
-    <cfRule type="colorScale" priority="15">
+  <conditionalFormatting sqref="AI22:AP22">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4969,8 +5107,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI29:AP29 AI32:AP32 AI26:AP26 AI20:AP20 AI17:AP17 AI14:AP14 AI11:AP11 AI8:AP8 AI5:AP5">
-    <cfRule type="colorScale" priority="14">
+  <conditionalFormatting sqref="AI23:AP23">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4981,8 +5119,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI33:AP33 AI30:AP30 AI6:AP6 AI9:AP9 AI12:AP12 AI15:AP15 AI18:AP18 AI21:AP21 AI27:AP27">
-    <cfRule type="colorScale" priority="13">
+  <conditionalFormatting sqref="AI24:AP24">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4993,7 +5131,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA22:AH22">
+  <conditionalFormatting sqref="H28:I28">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -5005,7 +5143,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA23:AH23">
+  <conditionalFormatting sqref="H29:I29">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -5017,7 +5155,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA24:AH24">
+  <conditionalFormatting sqref="H30:I30">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -5029,7 +5167,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI22:AP22">
+  <conditionalFormatting sqref="J28">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -5041,7 +5179,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI23:AP23">
+  <conditionalFormatting sqref="J29">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -5053,7 +5191,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI24:AP24">
+  <conditionalFormatting sqref="J30">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -5083,64 +5221,87 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231F6EA-36D1-4E59-A8F8-5864590C36B9}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="59">
-        <v>54.6</v>
-      </c>
-      <c r="C1" s="59">
-        <v>40</v>
-      </c>
-      <c r="D1" s="59">
-        <v>38.9</v>
-      </c>
-      <c r="E1" s="59">
-        <v>23.1</v>
-      </c>
+    <row r="1" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="67"/>
+      <c r="E1" s="44"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="61">
-        <v>69.8</v>
-      </c>
-      <c r="C2" s="61">
-        <v>56.4</v>
-      </c>
-      <c r="D2" s="61">
-        <v>52.4</v>
-      </c>
-      <c r="E2" s="61">
-        <v>31.1</v>
-      </c>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="66">
+        <v>66.2</v>
+      </c>
+      <c r="C2" s="66">
+        <v>81</v>
+      </c>
+      <c r="D2" s="66">
+        <v>0.3</v>
+      </c>
+      <c r="E2" s="45"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="59">
-        <v>0.52</v>
-      </c>
-      <c r="C3" s="59">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="66">
+        <v>42.8</v>
+      </c>
+      <c r="C3" s="66">
+        <v>62.8</v>
+      </c>
+      <c r="D3" s="66">
         <v>0.4</v>
       </c>
-      <c r="D3" s="59">
-        <v>0.36</v>
-      </c>
-      <c r="E3" s="59">
-        <v>0.32</v>
+      <c r="E3" s="44"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="66">
+        <v>35.5</v>
+      </c>
+      <c r="C4" s="66">
+        <v>52.9</v>
+      </c>
+      <c r="D4" s="66">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="66">
+        <v>23.8</v>
+      </c>
+      <c r="C5" s="66">
+        <v>32.5</v>
+      </c>
+      <c r="D5" s="66">
+        <v>0.37</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>